<commit_message>
Atualização pós levantamento até contrato.
</commit_message>
<xml_diff>
--- a/vbn/cards/Cards_AXIAL-Qualidade.xlsx
+++ b/vbn/cards/Cards_AXIAL-Qualidade.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18600" windowHeight="7695" activeTab="2"/>
+    <workbookView windowWidth="18600" windowHeight="7695" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PI" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125">
   <si>
     <t>Partes Interessadas</t>
   </si>
@@ -154,6 +154,21 @@
     <t>07-Estoque</t>
   </si>
   <si>
+    <t>08-Compras</t>
+  </si>
+  <si>
+    <t>09-Acopanhamento Axial</t>
+  </si>
+  <si>
+    <t>Área inexistente de apoio da equipe de qualidade a todos os processos da Axial. (remo)</t>
+  </si>
+  <si>
+    <t>10-Cadastro de produto</t>
+  </si>
+  <si>
+    <t>Área na Axial responsável pelo tramite de um produto dentro do contexto da Axial, com as variações (material., equipamento e sub).</t>
+  </si>
+  <si>
     <t>Atividade de Negócio</t>
   </si>
   <si>
@@ -219,6 +234,15 @@
     <t>Realizada anualmente tem como objetivo gerar gatilhos de atividades acerca das diretrizes de qualidade adotadas pela Axial, desde a inspesão física climática, ambiental, sanitária e inspesão regulatória de fornecedores. Como atualização de rastreabilidade de ativos da empresa. Acompanhamento de satisfação e relacionamento com fornecedores e clientes. Análise de conformidade(estado, validade, posição de estoque, etc) dos produtos consignados nos estoque distribuídos da Axial(hospitais e outros) e estoque local. Necessariamente deve acontecer uma análise de lições aprendidas(SERÀ UM MACRO)</t>
   </si>
   <si>
+    <t>10-Iniciar pedido de compra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">É dado inicio no processo de pedido de compra, onde as áreas responsáveis </t>
+  </si>
+  <si>
+    <t>11-Cadastro de produtos</t>
+  </si>
+  <si>
     <t>Ação do Fluxo de Negócio</t>
   </si>
   <si>
@@ -244,7 +268,7 @@
     <t>01-Levantar regulamentação necessária</t>
   </si>
   <si>
-    <t>De acordo com o segmento do fornecedor, a equipe levanta quais exigências de regulamentação são elegíveis ao contexto do fornecedor para um determinado material. Estas exigências são analisadas pela equipe responsável na Axial, em seguida repassada para validação do fornecedor.</t>
+    <t>Caso o fornecedor, seja elegível a avaliação regulatória da RCD16-2013 ou equivalente(de acordo com o segmento do fornecedor) a equipe levanta quais exigências de regulamentação são elegíveis ao contexto do fornecedor para um determinado material. Estas exigências são analisadas pela equipe responsável na Axial, em seguida repassada para validação do fornecedor.</t>
   </si>
   <si>
     <t>N/A</t>
@@ -253,16 +277,87 @@
     <t>02-Enviar exigências ao fornecedor</t>
   </si>
   <si>
-    <t>As regulamentações levantadas pela equipe da Axial é enviada para o fornecedor pelos meios disponíveis, as exigências são enviadas com os devidos embasamentos. A equipe deve monitorar para que o fornecedor forneça um retorno em tempo hábil ao prazo máximo de aquisição.</t>
-  </si>
-  <si>
-    <t>o material em questão seja elegível</t>
+    <t>As regulamentações levantadas pela equipe da Axial é enviada para o fornecedor pelos meios disponíveis, as exigências são enviadas com os devidos embasamentos. A equipe deve monitorar para que o fornecedor forneça um retorno em tempo hábil ao prazo máximo de aquisição.
+As exigências são enviadas em formulário com modelos definidos pela Axial:
+- Checklist de documentação para cadastro: para devido preenchimento e anexos (docs);
+- Checklist de avaliação estrutural: onde a empresa certificará a Axial do comprimento de normativas quanto as condições de instalação fisica (exigidas pela resolução RDC16-2013 e segmentadas);
+- Checklist de atendimento a RDC16-2013: onde a empresa certificará a Axial do comprimento de normativas gerais da resolução RDC16-2013, exceto as diretrizes de estrutura fisica já vistas no checklist específico.</t>
+  </si>
+  <si>
+    <t>o material do fornecedor em questão seja elegível</t>
   </si>
   <si>
     <t>03-Analisar feedback do fornecedor</t>
   </si>
   <si>
+    <t>Equipe recebe, analisa e atualiza no sistema a documentação enviada pelo fornecedor.
+Uma vez validada a docuentação, o fornecedor estará apto a relação comercial com a axial.
+Nesse momento é possível criar/manter o contrato de relação d Axial com o fornecedor;
+**sub funcionalidade para armazenamento e controle de validade dos documentos enviados (a resolução exige que seja renovado anualmente e/ou período adequado a natureza do doc), a nível de sistema, pode ser enviado automáticamente.</t>
+  </si>
+  <si>
     <t>o fornecedor analisar e retornar</t>
+  </si>
+  <si>
+    <t>04-Enviar documentação regulatória ao fornecedor</t>
+  </si>
+  <si>
+    <t>Equipe responsável na Axial, prepara e envia documentação regulatória ao fornecedor. (contrato social, AFE (autorização de funcionamento especial), licença de funcionamento, licença de vigilância sanitária, etc)
+**acontacerá como fluxo paralelo ao solicitar exigências do fornecedor.</t>
+  </si>
+  <si>
+    <t>o fornecedor solicitar documentação</t>
+  </si>
+  <si>
+    <t>05-Receber contrato do fornecedor</t>
+  </si>
+  <si>
+    <t>Equipe de qualidade, recebe a analisa o contrato enviado pelo fornecedor, com a perspectiva de acompanhamento dos materiais e condições de relacionamento baseado nas normativas e etc.
+Em seguida a equipe encaminha para diretoria e consultoria jurídica.</t>
+  </si>
+  <si>
+    <t>o fornecedor enviar o contrato</t>
+  </si>
+  <si>
+    <t>06-Coletar tabela de preços</t>
+  </si>
+  <si>
+    <t>Equipe coleta do fornecedor a tabela de preços praticados para um determnado produto, para que seja utilizado como base de valores de um produto caadstrado no sistema.</t>
+  </si>
+  <si>
+    <t>07-Avaliação Jurídica do contrato</t>
+  </si>
+  <si>
+    <t>Equipe externa que avalia as codições jurídicas do contrato e atesta a validade.</t>
+  </si>
+  <si>
+    <t>07-Incluir o produto no sistema</t>
+  </si>
+  <si>
+    <t>Cadastra as informações básicas de um produto:
+- tipo do produto(material, equipamento, instrumental, acessórios);
+- fabricante, Divisão, linha, modelo, referência, etc;
+- dados tributários do produto, NCM;
+- custo, unidade comercial, moeda, valor de venda;
+- registro anvisa, classificação de risco, validade ou vigência do produto na Anvisa (**possibilitar integração com REST API da ANVISA, a necessidade é recorrente e pode gerar dados inconsistentes).</t>
+  </si>
+  <si>
+    <t>08-Criar Kit  Cirúrgico</t>
+  </si>
+  <si>
+    <t>Equipe monta um novo kit cirúrgico com os devidos produtos e quantidades. (Tratar kit com herança dos produtos de sua composição, inclusive validade/vigência, fabricante, divisão, linha, modelo, referência e etc.)</t>
+  </si>
+  <si>
+    <t>09-Criar Contrato</t>
+  </si>
+  <si>
+    <t>Equipe cria um objeto de contrato dentro do sistema, para estabelecer as diretrizes básicas entre um fornecedor com um determinado produto/conjunto de produtos e as expectativas da Axial enquanto consumidor intermediario.
+- Um contrato obrigatoriamente deve ter prazo de entrega do forncedor para um produto(ou conjunto);
+- Um contrato obrigatoriamente deve ter o preço acordado para um determinado produto;
+- Um contrato obrigatoriamente deve ter um prazo de pagamento acordado para o fornnecedor;
+- Um contrato obrigatoriamente deve ter um valor mínimo executável.
+- Um contrato tem um conjunto de regras/alertas (de acordo com a seleção, o comprotamento e obrigatoriedade é diferente);
+Possibilitando seleção de acordo com fornecedor e aplicabilidade.</t>
   </si>
   <si>
     <t>Expectativas da Área de Negócio</t>
@@ -407,12 +502,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,11 +540,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -460,39 +586,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -514,15 +610,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -536,34 +625,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -574,9 +640,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -590,19 +685,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -618,7 +706,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -630,19 +808,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -654,19 +844,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -678,61 +874,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -744,61 +886,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -901,11 +989,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -940,32 +1034,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -983,6 +1051,26 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -992,152 +1080,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1198,13 +1286,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1225,10 +1316,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1238,52 +1325,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1600,10 +1644,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -1618,61 +1662,61 @@
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="2" s="18" customFormat="1" spans="1:7">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="52"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
     </row>
     <row r="3" s="18" customFormat="1" spans="1:7">
-      <c r="A3" s="43"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="54"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
     </row>
     <row r="4" s="18" customFormat="1" spans="1:7">
-      <c r="A4" s="43"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="54"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
     </row>
     <row r="5" s="18" customFormat="1" spans="1:7">
-      <c r="A5" s="43"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="54"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
     </row>
     <row r="6" s="18" customFormat="1" spans="1:7">
-      <c r="A6" s="46"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="56"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
     </row>
     <row r="7" spans="5:7">
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="22" t="s">
@@ -1706,10 +1750,9 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C10"/>
       <c r="D10" s="18" t="s">
         <v>9</v>
       </c>
@@ -1721,7 +1764,7 @@
       <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
@@ -1735,10 +1778,10 @@
       <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1749,10 +1792,10 @@
       <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="36" t="s">
+      <c r="D13" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1763,10 +1806,10 @@
       <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1777,18 +1820,22 @@
       <c r="B15" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="16" spans="3:4">
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:D6"/>
   </mergeCells>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.314583333333333" footer="0.314583333333333"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
@@ -1800,13 +1847,13 @@
   <dimension ref="A1:G117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="27.8583333333333" customWidth="1"/>
-    <col min="2" max="2" width="16.5666666666667" customWidth="1"/>
+    <col min="2" max="2" width="23.125" customWidth="1"/>
     <col min="3" max="3" width="70.5666666666667" customWidth="1"/>
     <col min="4" max="4" width="9.14166666666667" customWidth="1"/>
   </cols>
@@ -1820,48 +1867,48 @@
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="37"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="36"/>
     </row>
     <row r="3" s="18" customFormat="1" spans="1:7">
-      <c r="A3" s="30"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="38"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" s="18" customFormat="1" spans="1:7">
-      <c r="A4" s="30"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="38"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" s="18" customFormat="1" spans="1:7">
-      <c r="A5" s="30"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="38"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" s="18" customFormat="1" spans="1:7">
-      <c r="A6" s="32"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="39"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="38"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="22" t="s">
@@ -1949,14 +1996,36 @@
       </c>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="3:3">
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="3:3">
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="3:3">
-      <c r="C18" s="2"/>
+    <row r="17" ht="25.5" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" ht="25.5" spans="1:3">
+      <c r="A18" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" s="2"/>
@@ -2260,11 +2329,11 @@
     <mergeCell ref="A2:G6"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A109">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A18;A9:A17;A19:A109">
       <formula1>PI!$A$9:$A$109</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.314583333333333" footer="0.314583333333333"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -2274,69 +2343,69 @@
   <sheetPr/>
   <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="27.8583333333333" customWidth="1"/>
-    <col min="2" max="2" width="16.5666666666667" customWidth="1"/>
+    <col min="2" max="2" width="21.875" customWidth="1"/>
     <col min="3" max="3" width="43.125" customWidth="1"/>
-    <col min="4" max="4" width="58.5666666666667" style="28" customWidth="1"/>
+    <col min="4" max="4" width="58.5666666666667" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" spans="1:1">
       <c r="A1" s="19" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" s="18" customFormat="1" spans="1:7">
       <c r="A2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
+        <v>49</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="37"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="36"/>
     </row>
     <row r="3" s="18" customFormat="1" spans="1:7">
-      <c r="A3" s="30"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="38"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" s="18" customFormat="1" spans="1:7">
-      <c r="A4" s="30"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="7"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="38"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" s="18" customFormat="1" spans="1:7">
-      <c r="A5" s="30"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="38"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" s="18" customFormat="1" spans="1:7">
-      <c r="A6" s="32"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="39"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="38"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="22" t="s">
@@ -2347,10 +2416,10 @@
         <v>AN</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" ht="102" spans="1:4">
@@ -2361,10 +2430,10 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" ht="25.5" spans="1:4">
@@ -2375,10 +2444,10 @@
         <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" ht="51" spans="1:4">
@@ -2389,24 +2458,24 @@
         <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" ht="63.75" spans="1:4">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
         <v>42</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" ht="76.5" spans="1:4">
@@ -2417,10 +2486,10 @@
         <v>33</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>56</v>
+        <v>60</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2431,10 +2500,10 @@
         <v>31</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2445,10 +2514,10 @@
         <v>31</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="35" t="s">
-        <v>58</v>
+        <v>64</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="16" ht="114.75" spans="1:4">
@@ -2459,397 +2528,323 @@
         <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="35" t="s">
-        <v>61</v>
+        <v>65</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="17" ht="127.5" spans="1:4">
-      <c r="A17" s="36" t="s">
+      <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4">
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="3:4">
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="3:4">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" ht="25.5" spans="1:4">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3">
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="3:4">
+    </row>
+    <row r="21" spans="3:3">
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="3:4">
+    </row>
+    <row r="22" spans="3:3">
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="3:4">
+    </row>
+    <row r="23" spans="3:3">
       <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="3:4">
+    </row>
+    <row r="24" spans="3:3">
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="3:4">
+    </row>
+    <row r="25" spans="3:3">
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="3:4">
+    </row>
+    <row r="26" spans="3:3">
       <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="3:4">
+    </row>
+    <row r="27" spans="3:3">
       <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="3:4">
+    </row>
+    <row r="28" spans="3:3">
       <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="3:4">
+    </row>
+    <row r="29" spans="3:3">
       <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="3:4">
+    </row>
+    <row r="30" spans="3:3">
       <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="3:4">
+    </row>
+    <row r="31" spans="3:3">
       <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="3:4">
+    </row>
+    <row r="32" spans="3:3">
       <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="3:4">
+    </row>
+    <row r="33" spans="3:3">
       <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="3:4">
+    </row>
+    <row r="34" spans="3:3">
       <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="3:4">
+    </row>
+    <row r="35" spans="3:3">
       <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="3:4">
+    </row>
+    <row r="36" spans="3:3">
       <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="3:4">
+    </row>
+    <row r="37" spans="3:3">
       <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="3:4">
+    </row>
+    <row r="38" spans="3:3">
       <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="3:4">
+    </row>
+    <row r="39" spans="3:3">
       <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="3:4">
+    </row>
+    <row r="40" spans="3:3">
       <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="3:4">
+    </row>
+    <row r="41" spans="3:3">
       <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="3:4">
+    </row>
+    <row r="42" spans="3:3">
       <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="3:4">
+    </row>
+    <row r="43" spans="3:3">
       <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="3:4">
+    </row>
+    <row r="44" spans="3:3">
       <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-    </row>
-    <row r="45" spans="3:4">
+    </row>
+    <row r="45" spans="3:3">
       <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="3:4">
+    </row>
+    <row r="46" spans="3:3">
       <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-    </row>
-    <row r="47" spans="3:4">
+    </row>
+    <row r="47" spans="3:3">
       <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-    </row>
-    <row r="48" spans="3:4">
+    </row>
+    <row r="48" spans="3:3">
       <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="3:4">
+    </row>
+    <row r="49" spans="3:3">
       <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-    </row>
-    <row r="50" spans="3:4">
+    </row>
+    <row r="50" spans="3:3">
       <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-    </row>
-    <row r="51" spans="3:4">
+    </row>
+    <row r="51" spans="3:3">
       <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-    </row>
-    <row r="52" spans="3:4">
+    </row>
+    <row r="52" spans="3:3">
       <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-    </row>
-    <row r="53" spans="3:4">
+    </row>
+    <row r="53" spans="3:3">
       <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-    </row>
-    <row r="54" spans="3:4">
+    </row>
+    <row r="54" spans="3:3">
       <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-    </row>
-    <row r="55" spans="3:4">
+    </row>
+    <row r="55" spans="3:3">
       <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-    </row>
-    <row r="56" spans="3:4">
+    </row>
+    <row r="56" spans="3:3">
       <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-    </row>
-    <row r="57" spans="3:4">
+    </row>
+    <row r="57" spans="3:3">
       <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-    </row>
-    <row r="58" spans="3:4">
+    </row>
+    <row r="58" spans="3:3">
       <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="3:4">
+    </row>
+    <row r="59" spans="3:3">
       <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-    </row>
-    <row r="60" spans="3:4">
+    </row>
+    <row r="60" spans="3:3">
       <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-    </row>
-    <row r="61" spans="3:4">
+    </row>
+    <row r="61" spans="3:3">
       <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-    </row>
-    <row r="62" spans="3:4">
+    </row>
+    <row r="62" spans="3:3">
       <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-    </row>
-    <row r="63" spans="3:4">
+    </row>
+    <row r="63" spans="3:3">
       <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-    </row>
-    <row r="64" spans="3:4">
+    </row>
+    <row r="64" spans="3:3">
       <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="3:4">
+    </row>
+    <row r="65" spans="3:3">
       <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="3:4">
+    </row>
+    <row r="66" spans="3:3">
       <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-    </row>
-    <row r="67" spans="3:4">
+    </row>
+    <row r="67" spans="3:3">
       <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-    </row>
-    <row r="68" spans="3:4">
+    </row>
+    <row r="68" spans="3:3">
       <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="3:4">
+    </row>
+    <row r="69" spans="3:3">
       <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-    </row>
-    <row r="70" spans="3:4">
+    </row>
+    <row r="70" spans="3:3">
       <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-    </row>
-    <row r="71" spans="3:4">
+    </row>
+    <row r="71" spans="3:3">
       <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
-    </row>
-    <row r="72" spans="3:4">
+    </row>
+    <row r="72" spans="3:3">
       <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-    </row>
-    <row r="73" spans="3:4">
+    </row>
+    <row r="73" spans="3:3">
       <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-    </row>
-    <row r="74" spans="3:4">
+    </row>
+    <row r="74" spans="3:3">
       <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-    </row>
-    <row r="75" spans="3:4">
+    </row>
+    <row r="75" spans="3:3">
       <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-    </row>
-    <row r="76" spans="3:4">
+    </row>
+    <row r="76" spans="3:3">
       <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
-    </row>
-    <row r="77" spans="3:4">
+    </row>
+    <row r="77" spans="3:3">
       <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
-    </row>
-    <row r="78" spans="3:4">
+    </row>
+    <row r="78" spans="3:3">
       <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
-    </row>
-    <row r="79" spans="3:4">
+    </row>
+    <row r="79" spans="3:3">
       <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-    </row>
-    <row r="80" spans="3:4">
+    </row>
+    <row r="80" spans="3:3">
       <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-    </row>
-    <row r="81" spans="3:4">
+    </row>
+    <row r="81" spans="3:3">
       <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
-    </row>
-    <row r="82" spans="3:4">
+    </row>
+    <row r="82" spans="3:3">
       <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
-    </row>
-    <row r="83" spans="3:4">
+    </row>
+    <row r="83" spans="3:3">
       <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
-    </row>
-    <row r="84" spans="3:4">
+    </row>
+    <row r="84" spans="3:3">
       <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-    </row>
-    <row r="85" spans="3:4">
+    </row>
+    <row r="85" spans="3:3">
       <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
-    </row>
-    <row r="86" spans="3:4">
+    </row>
+    <row r="86" spans="3:3">
       <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
-    </row>
-    <row r="87" spans="3:4">
+    </row>
+    <row r="87" spans="3:3">
       <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
-    </row>
-    <row r="88" spans="3:4">
+    </row>
+    <row r="88" spans="3:3">
       <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
-    </row>
-    <row r="89" spans="3:4">
+    </row>
+    <row r="89" spans="3:3">
       <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
-    </row>
-    <row r="90" spans="3:4">
+    </row>
+    <row r="90" spans="3:3">
       <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
-    </row>
-    <row r="91" spans="3:4">
+    </row>
+    <row r="91" spans="3:3">
       <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
-    </row>
-    <row r="92" spans="3:4">
+    </row>
+    <row r="92" spans="3:3">
       <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-    </row>
-    <row r="93" spans="3:4">
+    </row>
+    <row r="93" spans="3:3">
       <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
-    </row>
-    <row r="94" spans="3:4">
+    </row>
+    <row r="94" spans="3:3">
       <c r="C94" s="2"/>
-      <c r="D94" s="2"/>
-    </row>
-    <row r="95" spans="3:4">
+    </row>
+    <row r="95" spans="3:3">
       <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
-    </row>
-    <row r="96" spans="3:4">
+    </row>
+    <row r="96" spans="3:3">
       <c r="C96" s="2"/>
-      <c r="D96" s="2"/>
-    </row>
-    <row r="97" spans="3:4">
+    </row>
+    <row r="97" spans="3:3">
       <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
-    </row>
-    <row r="98" spans="3:4">
+    </row>
+    <row r="98" spans="3:3">
       <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
-    </row>
-    <row r="99" spans="3:4">
+    </row>
+    <row r="99" spans="3:3">
       <c r="C99" s="2"/>
-      <c r="D99" s="2"/>
-    </row>
-    <row r="100" spans="3:4">
+    </row>
+    <row r="100" spans="3:3">
       <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
-    </row>
-    <row r="101" spans="3:4">
+    </row>
+    <row r="101" spans="3:3">
       <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
-    </row>
-    <row r="102" spans="3:4">
+    </row>
+    <row r="102" spans="3:3">
       <c r="C102" s="2"/>
-      <c r="D102" s="2"/>
-    </row>
-    <row r="103" spans="3:4">
+    </row>
+    <row r="103" spans="3:3">
       <c r="C103" s="2"/>
-      <c r="D103" s="2"/>
-    </row>
-    <row r="104" spans="3:4">
+    </row>
+    <row r="104" spans="3:3">
       <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
-    </row>
-    <row r="105" spans="3:4">
+    </row>
+    <row r="105" spans="3:3">
       <c r="C105" s="2"/>
-      <c r="D105" s="2"/>
-    </row>
-    <row r="106" spans="3:4">
+    </row>
+    <row r="106" spans="3:3">
       <c r="C106" s="2"/>
-      <c r="D106" s="2"/>
-    </row>
-    <row r="107" spans="3:4">
+    </row>
+    <row r="107" spans="3:3">
       <c r="C107" s="2"/>
-      <c r="D107" s="2"/>
-    </row>
-    <row r="108" spans="3:4">
+    </row>
+    <row r="108" spans="3:3">
       <c r="C108" s="2"/>
-      <c r="D108" s="2"/>
-    </row>
-    <row r="109" spans="3:4">
+    </row>
+    <row r="109" spans="3:3">
       <c r="C109" s="2"/>
-      <c r="D109" s="2"/>
-    </row>
-    <row r="110" spans="3:4">
+    </row>
+    <row r="110" spans="3:3">
       <c r="C110" s="2"/>
-      <c r="D110" s="2"/>
     </row>
     <row r="111" spans="3:3">
       <c r="C111" s="2"/>
@@ -2887,7 +2882,7 @@
       <formula1>PI!$A$9:$A$109</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.314583333333333" footer="0.314583333333333"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
@@ -2896,10 +2891,12 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="7"/>
@@ -2916,23 +2913,23 @@
   <sheetData>
     <row r="1" ht="34.5" spans="1:8">
       <c r="A1" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+        <v>72</v>
+      </c>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" s="1" customFormat="1" ht="15" customHeight="1" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="12"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:8">
       <c r="A3" s="6"/>
@@ -2940,9 +2937,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="13"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:8">
       <c r="A4" s="6"/>
@@ -2950,9 +2947,9 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="13"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:8">
       <c r="A5" s="6"/>
@@ -2960,9 +2957,9 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="13"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:8">
       <c r="A6" s="8"/>
@@ -2970,14 +2967,14 @@
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="6:8">
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
     </row>
     <row r="8" ht="25.5" spans="1:8">
       <c r="A8" s="10" t="s">
@@ -2988,23 +2985,23 @@
         <v>AN</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H8" s="26"/>
-    </row>
-    <row r="9" ht="63.75" spans="1:6">
+        <v>78</v>
+      </c>
+      <c r="H8" s="27"/>
+    </row>
+    <row r="9" ht="76.5" spans="1:6">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -3012,19 +3009,19 @@
         <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" ht="63.75" spans="1:7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" ht="216.75" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -3032,22 +3029,22 @@
         <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>75</v>
+        <v>82</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>83</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" ht="25.5" spans="1:7">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" ht="153" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -3055,38 +3052,324 @@
         <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" ht="15" customHeight="1"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" ht="76.5" spans="1:7">
+      <c r="A12" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" ht="63.75" spans="1:7">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" ht="38.25" spans="1:7">
+      <c r="A14" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" ht="25.5" spans="1:5">
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" ht="114.75" spans="1:5">
+      <c r="A16" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" ht="51" spans="1:6">
+      <c r="A17" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" ht="204" spans="1:5">
+      <c r="A18" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" s="26"/>
+    </row>
+    <row r="20" spans="3:3">
+      <c r="C20" s="26"/>
+    </row>
+    <row r="21" spans="3:3">
+      <c r="C21" s="26"/>
+    </row>
+    <row r="22" spans="3:3">
+      <c r="C22" s="26"/>
+    </row>
+    <row r="23" spans="3:3">
+      <c r="C23" s="26"/>
+    </row>
+    <row r="24" spans="3:3">
+      <c r="C24" s="26"/>
+    </row>
+    <row r="25" spans="3:3">
+      <c r="C25" s="26"/>
+    </row>
+    <row r="26" spans="3:3">
+      <c r="C26" s="26"/>
+    </row>
+    <row r="27" spans="3:3">
+      <c r="C27" s="26"/>
+    </row>
+    <row r="28" spans="3:3">
+      <c r="C28" s="26"/>
+    </row>
+    <row r="29" spans="3:3">
+      <c r="C29" s="26"/>
+    </row>
+    <row r="30" spans="3:3">
+      <c r="C30" s="26"/>
+    </row>
+    <row r="31" spans="3:3">
+      <c r="C31" s="26"/>
+    </row>
+    <row r="32" spans="3:3">
+      <c r="C32" s="26"/>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="26"/>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="26"/>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" s="26"/>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" s="26"/>
+    </row>
+    <row r="37" spans="3:3">
+      <c r="C37" s="26"/>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" s="26"/>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" s="26"/>
+    </row>
+    <row r="40" spans="3:3">
+      <c r="C40" s="26"/>
+    </row>
+    <row r="41" spans="3:3">
+      <c r="C41" s="26"/>
+    </row>
+    <row r="42" spans="3:3">
+      <c r="C42" s="26"/>
+    </row>
+    <row r="43" spans="3:3">
+      <c r="C43" s="26"/>
+    </row>
+    <row r="44" spans="3:3">
+      <c r="C44" s="26"/>
+    </row>
+    <row r="45" spans="3:3">
+      <c r="C45" s="26"/>
+    </row>
+    <row r="46" spans="3:3">
+      <c r="C46" s="26"/>
+    </row>
+    <row r="47" spans="3:3">
+      <c r="C47" s="26"/>
+    </row>
+    <row r="48" spans="3:3">
+      <c r="C48" s="26"/>
+    </row>
+    <row r="49" spans="3:3">
+      <c r="C49" s="26"/>
+    </row>
+    <row r="50" spans="3:3">
+      <c r="C50" s="26"/>
+    </row>
+    <row r="51" spans="3:3">
+      <c r="C51" s="26"/>
+    </row>
+    <row r="52" spans="3:3">
+      <c r="C52" s="26"/>
+    </row>
+    <row r="53" spans="3:3">
+      <c r="C53" s="26"/>
+    </row>
+    <row r="54" spans="3:3">
+      <c r="C54" s="26"/>
+    </row>
+    <row r="55" spans="3:3">
+      <c r="C55" s="26"/>
+    </row>
+    <row r="56" spans="3:3">
+      <c r="C56" s="26"/>
+    </row>
+    <row r="57" spans="3:3">
+      <c r="C57" s="26"/>
+    </row>
+    <row r="58" spans="3:3">
+      <c r="C58" s="26"/>
+    </row>
+    <row r="59" spans="3:3">
+      <c r="C59" s="26"/>
+    </row>
+    <row r="60" spans="3:3">
+      <c r="C60" s="26"/>
+    </row>
+    <row r="61" spans="3:3">
+      <c r="C61" s="26"/>
+    </row>
+    <row r="62" spans="3:3">
+      <c r="C62" s="26"/>
+    </row>
+    <row r="63" spans="3:3">
+      <c r="C63" s="26"/>
+    </row>
+    <row r="64" spans="3:3">
+      <c r="C64" s="26"/>
+    </row>
+    <row r="65" spans="3:3">
+      <c r="C65" s="26"/>
+    </row>
+    <row r="66" spans="3:3">
+      <c r="C66" s="26"/>
+    </row>
+    <row r="67" spans="3:3">
+      <c r="C67" s="26"/>
+    </row>
+    <row r="68" spans="3:3">
+      <c r="C68" s="26"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:E6"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9:G109">
-      <formula1>$D$9:$D$109</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C11;C16:C109">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12;C13;C14;C15;C18;C9:C11;C16:C17;C19:C68;C69:C110">
       <formula1>ATVN!$C$9:$C$110</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B109">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12;B13;B14;B15;B16;B17;B18;B9:B11;B19:B110">
       <formula1>AN!$B$9:$B$109</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A109">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G14;G9:G13;G15:G110">
+      <formula1>$D$9:$D$110</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A12;A13;A14;A15;A16;A17;A18;A9:A11;A19:A110">
       <formula1>PI!$A$9:$A$109</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.314583333333333" footer="0.314583333333333"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
@@ -3112,12 +3395,12 @@
   <sheetData>
     <row r="1" ht="34.5" spans="1:1">
       <c r="A1" s="25" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:7">
       <c r="A2" s="4" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -3171,10 +3454,10 @@
         <v>AN</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" ht="25.5" spans="1:4">
@@ -3185,10 +3468,10 @@
         <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" ht="25.5" spans="1:4">
@@ -3199,10 +3482,10 @@
         <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -3220,7 +3503,7 @@
       <formula1>PI!$A$9:$A$109</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.314583333333333" footer="0.314583333333333"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
@@ -3245,7 +3528,7 @@
   <sheetData>
     <row r="1" ht="17.25" spans="1:8">
       <c r="A1" s="19" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
@@ -3255,7 +3538,7 @@
     </row>
     <row r="2" s="18" customFormat="1" ht="15" customHeight="1" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="12"/>
@@ -3321,7 +3604,7 @@
         <v>AN</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="20"/>
@@ -3681,7 +3964,7 @@
       <formula1>PI!$A$9:$A$109</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.314583333333333" footer="0.314583333333333"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -3711,12 +3994,12 @@
   <sheetData>
     <row r="1" ht="17.25" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="15" customHeight="1" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -3725,7 +4008,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="12"/>
       <c r="I2" s="16" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:9">
@@ -3737,7 +4020,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="13"/>
       <c r="I3" s="17" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:9">
@@ -3749,7 +4032,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="13"/>
       <c r="I4" s="17" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:7">
@@ -3808,30 +4091,30 @@
     </row>
     <row r="11" ht="25.5" spans="1:7">
       <c r="A11" s="10" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" ht="89.25" spans="1:7">
       <c r="A12" s="11" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>33</v>
@@ -3840,16 +4123,16 @@
         <v>6</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:1">
@@ -4151,11 +4434,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12:F109">
       <formula1>ATVN!$C$9:$C$110</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12:E109">
-      <formula1>AFN!$D$9:$D$109</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:B112">
       <formula1>AN!$B$9:$B$109</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12:E109">
+      <formula1>AFN!$D$9:$D$110</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:D109">
       <formula1>$I$2:$I$4</formula1>
@@ -4164,7 +4447,7 @@
       <formula1>PI!$A$9:$A$109</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.314583333333333" footer="0.314583333333333"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Ajuste da lista de requisitos da solução de regulatório.
</commit_message>
<xml_diff>
--- a/vbn/cards/Cards_AXIAL-Qualidade.xlsx
+++ b/vbn/cards/Cards_AXIAL-Qualidade.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18600" windowHeight="7695" activeTab="3"/>
+    <workbookView windowWidth="19890" windowHeight="8415" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="PI" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131">
   <si>
     <t>Partes Interessadas</t>
   </si>
@@ -483,7 +483,7 @@
     <t>Prioridade</t>
   </si>
   <si>
-    <t>para que seja possível realizar (ATVN)</t>
+    <t>para que seja possível (EXPEC)</t>
   </si>
   <si>
     <t>este requisito é considerado completo apenas se</t>
@@ -492,9 +492,25 @@
     <t>01</t>
   </si>
   <si>
-    <t>For possível ter uma lista de regulamentações associadas ao material em análise;
-For possível que uma análise regulatória seja continuada posteriormente;
-For possível reutilizar uma análise anterior.</t>
+    <t>For possível ter uma lista de regulamentações associadas ao material em análise.</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>For possível que uma análise regulatória do fornecedor seja continuada posteriormente.</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>For possível reutilizar uma análise anterior de qualquer fornecedor.</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>For possível gerar um relatório da análise regulatória de um ou mais fornecedores.</t>
   </si>
 </sst>
 </file>
@@ -503,9 +519,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -548,8 +564,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -557,7 +574,30 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -572,38 +612,30 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -625,11 +657,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -648,39 +693,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -706,13 +722,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -724,13 +734,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -742,19 +776,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -766,31 +812,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,37 +842,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -850,43 +878,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1004,6 +1020,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1015,21 +1040,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1063,169 +1073,175 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1256,6 +1272,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1286,18 +1308,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1325,7 +1341,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1644,7 +1659,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
@@ -1659,76 +1674,76 @@
   </cols>
   <sheetData>
     <row r="1" ht="17.25" spans="1:7">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-    </row>
-    <row r="2" s="18" customFormat="1" spans="1:7">
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+    </row>
+    <row r="2" s="20" customFormat="1" spans="1:7">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-    </row>
-    <row r="3" s="18" customFormat="1" spans="1:7">
+      <c r="D2" s="14"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+    </row>
+    <row r="3" s="20" customFormat="1" spans="1:7">
       <c r="A3" s="6"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-    </row>
-    <row r="4" s="18" customFormat="1" spans="1:7">
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+    </row>
+    <row r="4" s="20" customFormat="1" spans="1:7">
       <c r="A4" s="6"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-    </row>
-    <row r="5" s="18" customFormat="1" spans="1:7">
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+    </row>
+    <row r="5" s="20" customFormat="1" spans="1:7">
       <c r="A5" s="6"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-    </row>
-    <row r="6" s="18" customFormat="1" spans="1:7">
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+    </row>
+    <row r="6" s="20" customFormat="1" spans="1:7">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="5:7">
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="24" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1742,7 +1757,7 @@
       <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="20" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1750,10 +1765,10 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="20" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1826,10 +1841,6 @@
       <c r="D15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="3:4">
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1859,11 +1870,11 @@
   </cols>
   <sheetData>
     <row r="1" ht="17.25" spans="1:1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" s="18" customFormat="1" spans="1:7">
+    <row r="2" s="20" customFormat="1" spans="1:7">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
@@ -1874,7 +1885,7 @@
       <c r="F2" s="30"/>
       <c r="G2" s="36"/>
     </row>
-    <row r="3" s="18" customFormat="1" spans="1:7">
+    <row r="3" s="20" customFormat="1" spans="1:7">
       <c r="A3" s="31"/>
       <c r="B3" s="32"/>
       <c r="C3" s="32"/>
@@ -1883,7 +1894,7 @@
       <c r="F3" s="32"/>
       <c r="G3" s="37"/>
     </row>
-    <row r="4" s="18" customFormat="1" spans="1:7">
+    <row r="4" s="20" customFormat="1" spans="1:7">
       <c r="A4" s="31"/>
       <c r="B4" s="32"/>
       <c r="C4" s="32"/>
@@ -1892,7 +1903,7 @@
       <c r="F4" s="32"/>
       <c r="G4" s="37"/>
     </row>
-    <row r="5" s="18" customFormat="1" spans="1:7">
+    <row r="5" s="20" customFormat="1" spans="1:7">
       <c r="A5" s="31"/>
       <c r="B5" s="32"/>
       <c r="C5" s="32"/>
@@ -1901,7 +1912,7 @@
       <c r="F5" s="32"/>
       <c r="G5" s="37"/>
     </row>
-    <row r="6" s="18" customFormat="1" spans="1:7">
+    <row r="6" s="20" customFormat="1" spans="1:7">
       <c r="A6" s="33"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
@@ -1911,16 +1922,16 @@
       <c r="G6" s="38"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="24" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="23"/>
+      <c r="D8" s="25"/>
     </row>
     <row r="9" ht="25.5" spans="1:4">
       <c r="A9" t="s">
@@ -1932,7 +1943,7 @@
       <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="18"/>
+      <c r="D9" s="20"/>
     </row>
     <row r="10" ht="25.5" spans="1:3">
       <c r="A10" t="s">
@@ -2017,7 +2028,7 @@
       </c>
     </row>
     <row r="18" ht="25.5" spans="1:3">
-      <c r="A18" s="39" t="s">
+      <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18" t="s">
@@ -2356,11 +2367,11 @@
   </cols>
   <sheetData>
     <row r="1" ht="17.25" spans="1:1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" s="18" customFormat="1" spans="1:7">
+    <row r="2" s="20" customFormat="1" spans="1:7">
       <c r="A2" s="4" t="s">
         <v>49</v>
       </c>
@@ -2371,7 +2382,7 @@
       <c r="F2" s="30"/>
       <c r="G2" s="36"/>
     </row>
-    <row r="3" s="18" customFormat="1" spans="1:7">
+    <row r="3" s="20" customFormat="1" spans="1:7">
       <c r="A3" s="31"/>
       <c r="B3" s="32"/>
       <c r="C3" s="32"/>
@@ -2380,7 +2391,7 @@
       <c r="F3" s="32"/>
       <c r="G3" s="37"/>
     </row>
-    <row r="4" s="18" customFormat="1" spans="1:7">
+    <row r="4" s="20" customFormat="1" spans="1:7">
       <c r="A4" s="31"/>
       <c r="B4" s="32"/>
       <c r="C4" s="32"/>
@@ -2389,7 +2400,7 @@
       <c r="F4" s="32"/>
       <c r="G4" s="37"/>
     </row>
-    <row r="5" s="18" customFormat="1" spans="1:7">
+    <row r="5" s="20" customFormat="1" spans="1:7">
       <c r="A5" s="31"/>
       <c r="B5" s="32"/>
       <c r="C5" s="32"/>
@@ -2398,7 +2409,7 @@
       <c r="F5" s="32"/>
       <c r="G5" s="37"/>
     </row>
-    <row r="6" s="18" customFormat="1" spans="1:7">
+    <row r="6" s="20" customFormat="1" spans="1:7">
       <c r="A6" s="33"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
@@ -2408,14 +2419,14 @@
       <c r="G6" s="38"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="22" t="str">
+      <c r="B8" s="24" t="str">
         <f>"AN"</f>
         <v>AN</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="24" t="s">
         <v>48</v>
       </c>
       <c r="D8" s="10" t="s">
@@ -2891,9 +2902,9 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="C1" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
@@ -2912,12 +2923,12 @@
   </cols>
   <sheetData>
     <row r="1" ht="34.5" spans="1:8">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" s="1" customFormat="1" ht="15" customHeight="1" spans="1:8">
       <c r="A2" s="4" t="s">
@@ -2926,55 +2937,55 @@
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:8">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:8">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:8">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:8">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
     </row>
     <row r="7" spans="6:8">
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" ht="25.5" spans="1:8">
       <c r="A8" s="10" t="s">
@@ -2999,7 +3010,7 @@
       <c r="G8" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="H8" s="27"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" ht="76.5" spans="1:6">
       <c r="A9" s="2" t="s">
@@ -3034,7 +3045,7 @@
       <c r="D10" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="1" t="s">
         <v>83</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -3068,13 +3079,13 @@
       </c>
     </row>
     <row r="12" ht="76.5" spans="1:7">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -3097,7 +3108,7 @@
       <c r="B13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -3114,13 +3125,13 @@
       </c>
     </row>
     <row r="14" ht="38.25" spans="1:7">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -3129,17 +3140,14 @@
       <c r="E14" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="2" t="s">
         <v>93</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" ht="25.5" spans="1:5">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
+    <row r="15" ht="25.5" spans="4:5">
       <c r="D15" s="2" t="s">
         <v>96</v>
       </c>
@@ -3148,13 +3156,13 @@
       </c>
     </row>
     <row r="16" ht="114.75" spans="1:5">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -3165,13 +3173,13 @@
       </c>
     </row>
     <row r="17" ht="51" spans="1:6">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -3185,13 +3193,13 @@
       </c>
     </row>
     <row r="18" ht="204" spans="1:5">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -3200,156 +3208,6 @@
       <c r="E18" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="19" spans="3:3">
-      <c r="C19" s="26"/>
-    </row>
-    <row r="20" spans="3:3">
-      <c r="C20" s="26"/>
-    </row>
-    <row r="21" spans="3:3">
-      <c r="C21" s="26"/>
-    </row>
-    <row r="22" spans="3:3">
-      <c r="C22" s="26"/>
-    </row>
-    <row r="23" spans="3:3">
-      <c r="C23" s="26"/>
-    </row>
-    <row r="24" spans="3:3">
-      <c r="C24" s="26"/>
-    </row>
-    <row r="25" spans="3:3">
-      <c r="C25" s="26"/>
-    </row>
-    <row r="26" spans="3:3">
-      <c r="C26" s="26"/>
-    </row>
-    <row r="27" spans="3:3">
-      <c r="C27" s="26"/>
-    </row>
-    <row r="28" spans="3:3">
-      <c r="C28" s="26"/>
-    </row>
-    <row r="29" spans="3:3">
-      <c r="C29" s="26"/>
-    </row>
-    <row r="30" spans="3:3">
-      <c r="C30" s="26"/>
-    </row>
-    <row r="31" spans="3:3">
-      <c r="C31" s="26"/>
-    </row>
-    <row r="32" spans="3:3">
-      <c r="C32" s="26"/>
-    </row>
-    <row r="33" spans="3:3">
-      <c r="C33" s="26"/>
-    </row>
-    <row r="34" spans="3:3">
-      <c r="C34" s="26"/>
-    </row>
-    <row r="35" spans="3:3">
-      <c r="C35" s="26"/>
-    </row>
-    <row r="36" spans="3:3">
-      <c r="C36" s="26"/>
-    </row>
-    <row r="37" spans="3:3">
-      <c r="C37" s="26"/>
-    </row>
-    <row r="38" spans="3:3">
-      <c r="C38" s="26"/>
-    </row>
-    <row r="39" spans="3:3">
-      <c r="C39" s="26"/>
-    </row>
-    <row r="40" spans="3:3">
-      <c r="C40" s="26"/>
-    </row>
-    <row r="41" spans="3:3">
-      <c r="C41" s="26"/>
-    </row>
-    <row r="42" spans="3:3">
-      <c r="C42" s="26"/>
-    </row>
-    <row r="43" spans="3:3">
-      <c r="C43" s="26"/>
-    </row>
-    <row r="44" spans="3:3">
-      <c r="C44" s="26"/>
-    </row>
-    <row r="45" spans="3:3">
-      <c r="C45" s="26"/>
-    </row>
-    <row r="46" spans="3:3">
-      <c r="C46" s="26"/>
-    </row>
-    <row r="47" spans="3:3">
-      <c r="C47" s="26"/>
-    </row>
-    <row r="48" spans="3:3">
-      <c r="C48" s="26"/>
-    </row>
-    <row r="49" spans="3:3">
-      <c r="C49" s="26"/>
-    </row>
-    <row r="50" spans="3:3">
-      <c r="C50" s="26"/>
-    </row>
-    <row r="51" spans="3:3">
-      <c r="C51" s="26"/>
-    </row>
-    <row r="52" spans="3:3">
-      <c r="C52" s="26"/>
-    </row>
-    <row r="53" spans="3:3">
-      <c r="C53" s="26"/>
-    </row>
-    <row r="54" spans="3:3">
-      <c r="C54" s="26"/>
-    </row>
-    <row r="55" spans="3:3">
-      <c r="C55" s="26"/>
-    </row>
-    <row r="56" spans="3:3">
-      <c r="C56" s="26"/>
-    </row>
-    <row r="57" spans="3:3">
-      <c r="C57" s="26"/>
-    </row>
-    <row r="58" spans="3:3">
-      <c r="C58" s="26"/>
-    </row>
-    <row r="59" spans="3:3">
-      <c r="C59" s="26"/>
-    </row>
-    <row r="60" spans="3:3">
-      <c r="C60" s="26"/>
-    </row>
-    <row r="61" spans="3:3">
-      <c r="C61" s="26"/>
-    </row>
-    <row r="62" spans="3:3">
-      <c r="C62" s="26"/>
-    </row>
-    <row r="63" spans="3:3">
-      <c r="C63" s="26"/>
-    </row>
-    <row r="64" spans="3:3">
-      <c r="C64" s="26"/>
-    </row>
-    <row r="65" spans="3:3">
-      <c r="C65" s="26"/>
-    </row>
-    <row r="66" spans="3:3">
-      <c r="C66" s="26"/>
-    </row>
-    <row r="67" spans="3:3">
-      <c r="C67" s="26"/>
-    </row>
-    <row r="68" spans="3:3">
-      <c r="C68" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3381,7 +3239,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -3394,7 +3252,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="34.5" spans="1:1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3407,7 +3265,7 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="12"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:7">
       <c r="A3" s="6"/>
@@ -3416,7 +3274,7 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="13"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:7">
       <c r="A4" s="6"/>
@@ -3425,7 +3283,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="13"/>
+      <c r="G4" s="15"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:7">
       <c r="A5" s="6"/>
@@ -3434,7 +3292,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="13"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:7">
       <c r="A6" s="8"/>
@@ -3443,7 +3301,7 @@
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="14"/>
+      <c r="G6" s="16"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="10" t="s">
@@ -3527,90 +3385,90 @@
   </cols>
   <sheetData>
     <row r="1" ht="17.25" spans="1:8">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-    </row>
-    <row r="2" s="18" customFormat="1" ht="15" customHeight="1" spans="1:8">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+    </row>
+    <row r="2" s="20" customFormat="1" ht="15" customHeight="1" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>110</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="24"/>
-    </row>
-    <row r="3" s="18" customFormat="1" spans="1:8">
+      <c r="C2" s="14"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="26"/>
+    </row>
+    <row r="3" s="20" customFormat="1" spans="1:8">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="24"/>
-    </row>
-    <row r="4" s="18" customFormat="1" spans="1:8">
+      <c r="C3" s="15"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="26"/>
+    </row>
+    <row r="4" s="20" customFormat="1" spans="1:8">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="24"/>
-    </row>
-    <row r="5" s="18" customFormat="1" spans="1:8">
+      <c r="C4" s="15"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="26"/>
+    </row>
+    <row r="5" s="20" customFormat="1" spans="1:8">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="24"/>
-    </row>
-    <row r="6" s="18" customFormat="1" spans="1:8">
+      <c r="C5" s="15"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="26"/>
+    </row>
+    <row r="6" s="20" customFormat="1" spans="1:8">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="24"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="4:8">
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="22" t="str">
+      <c r="B8" s="24" t="str">
         <f>"AN"</f>
         <v>AN</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
@@ -3620,7 +3478,7 @@
         <v>31</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="18"/>
+      <c r="D9" s="20"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
@@ -3974,19 +3832,19 @@
   <sheetPr/>
   <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="7.70833333333333" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5666666666667" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.425" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.8583333333333" style="2" customWidth="1"/>
+    <col min="1" max="1" width="5.73333333333333" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.1416666666667" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.4666666666667" style="2" customWidth="1"/>
+    <col min="4" max="4" width="29.85" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.375" style="2" customWidth="1"/>
     <col min="6" max="6" width="35" style="2" customWidth="1"/>
-    <col min="7" max="7" width="34.5666666666667" style="2" customWidth="1"/>
+    <col min="7" max="7" width="42.0583333333333" style="2" customWidth="1"/>
     <col min="8" max="8" width="11.425" style="2" customWidth="1"/>
     <col min="9" max="9" width="9.14166666666667" style="2" hidden="1" customWidth="1"/>
     <col min="10" max="16384" width="9.14166666666667" style="2"/>
@@ -4006,8 +3864,8 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="12"/>
-      <c r="I2" s="16" t="s">
+      <c r="G2" s="14"/>
+      <c r="I2" s="18" t="s">
         <v>114</v>
       </c>
     </row>
@@ -4018,8 +3876,8 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="13"/>
-      <c r="I3" s="17" t="s">
+      <c r="G3" s="15"/>
+      <c r="I3" s="19" t="s">
         <v>115</v>
       </c>
     </row>
@@ -4030,8 +3888,8 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="13"/>
-      <c r="I4" s="17" t="s">
+      <c r="G4" s="15"/>
+      <c r="I4" s="19" t="s">
         <v>116</v>
       </c>
     </row>
@@ -4042,7 +3900,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="13"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:7">
       <c r="A6" s="6"/>
@@ -4051,7 +3909,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="13"/>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:7">
       <c r="A7" s="6"/>
@@ -4060,7 +3918,7 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="13"/>
+      <c r="G7" s="15"/>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:7">
       <c r="A8" s="6"/>
@@ -4069,7 +3927,7 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="13"/>
+      <c r="G8" s="15"/>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:7">
       <c r="A9" s="8"/>
@@ -4078,7 +3936,7 @@
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="14"/>
+      <c r="G9" s="16"/>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:7">
       <c r="A10" s="7"/>
@@ -4112,7 +3970,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" ht="89.25" spans="1:7">
+    <row r="12" ht="38.25" spans="1:7">
       <c r="A12" s="11" t="s">
         <v>123</v>
       </c>
@@ -4129,20 +3987,80 @@
         <v>79</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G12" s="17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="11"/>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="11"/>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="11"/>
+    <row r="13" ht="38.25" spans="1:7">
+      <c r="A13" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" ht="38.25" spans="1:7">
+      <c r="A14" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" ht="38.25" spans="1:7">
+      <c r="A15" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="11"/>
@@ -4430,20 +4348,23 @@
   <mergeCells count="1">
     <mergeCell ref="A2:G9"/>
   </mergeCells>
-  <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12:F109">
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12;F13;F14;F15">
+      <formula1>EXPEC!$D$9:$D$100</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12;B13;B14;B15;B16:B112">
+      <formula1>AN!$B$9:$B$109</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12;E13;E14;E15;E16:E109">
+      <formula1>AFN!$D$9:$D$110</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F16:F109">
       <formula1>ATVN!$C$9:$C$110</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:B112">
-      <formula1>AN!$B$9:$B$109</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12:E109">
-      <formula1>AFN!$D$9:$D$110</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:D109">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12;D13;D14;D15;D16:D109">
       <formula1>$I$2:$I$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A14:A107;C12:C112">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12;C13;C14;C15;A16:A107;C16:C112">
       <formula1>PI!$A$9:$A$109</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Inclusão de doc de visão e ajuste emplanilha de cards
</commit_message>
<xml_diff>
--- a/vbn/cards/Cards_AXIAL-Qualidade.xlsx
+++ b/vbn/cards/Cards_AXIAL-Qualidade.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="8415" activeTab="6"/>
+    <workbookView windowWidth="19890" windowHeight="8415" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PI" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,15 @@
     <sheet name="PROB" sheetId="6" r:id="rId6"/>
     <sheet name="RS" sheetId="7" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ATVN!$A$8:$C$17</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125">
   <si>
     <t>Partes Interessadas</t>
   </si>
@@ -42,7 +45,7 @@
     <t>Nível de envolvimento na solução</t>
   </si>
   <si>
-    <t>01-Axial/Gestão da Qualidade</t>
+    <t>Axial/Gestão da Qualidade (QA)</t>
   </si>
   <si>
     <t>Mychelle</t>
@@ -54,13 +57,16 @@
     <t>N3</t>
   </si>
   <si>
-    <t>03-Axial/Logística</t>
+    <t>Axial/Logística (LOG)</t>
   </si>
   <si>
     <t>Mychelle/Dionísio</t>
   </si>
   <si>
-    <t>04-Axial/Financeiro/Orçamento</t>
+    <t>Contribuinte para o tema logistica</t>
+  </si>
+  <si>
+    <t>Axial/Financeiro (FIN)</t>
   </si>
   <si>
     <t>Dionísio</t>
@@ -69,34 +75,25 @@
     <t>Contribuinte para o tema orçamento</t>
   </si>
   <si>
-    <t>05-Axial/Financeiro/Faturamento</t>
-  </si>
-  <si>
     <t>Rosangela</t>
   </si>
   <si>
     <t>Contribuinte para o tema faturamento</t>
   </si>
   <si>
-    <t>06-Axial/Financeiro</t>
-  </si>
-  <si>
     <t>Rosalyne</t>
   </si>
   <si>
     <t>Contribuinte para o tema financeiro</t>
   </si>
   <si>
-    <t>07-Axial/Logística/Distribuição</t>
-  </si>
-  <si>
     <t>Humberto/Tiago</t>
   </si>
   <si>
     <t>Contribuinte para o tema distribuição externa</t>
   </si>
   <si>
-    <t>08-Axial/Comercial</t>
+    <t>Axial/Comercial (COM)</t>
   </si>
   <si>
     <t>Jacob/Dionísio</t>
@@ -109,6 +106,7 @@
   </si>
   <si>
     <t xml:space="preserve">1. Para preenchimento do card das áreas de negócio (AN), preencha o campo descrição com informações que explanem resumidamente a responsabilidade da área.
+2. Uma AN necessariamente será suportada por uma parte interessada.
 </t>
   </si>
   <si>
@@ -118,129 +116,118 @@
     <t>Descrição da área de negócio</t>
   </si>
   <si>
-    <t>01-Qualidade</t>
+    <t>Qualidade Assegurada</t>
   </si>
   <si>
     <t>Área na Axial responsável pelo fomento e garantia da qualidade de processo, produtos e serviços prestados pela empresa.</t>
   </si>
   <si>
-    <t>02-Regulatório</t>
+    <t>Regulatório</t>
   </si>
   <si>
     <t>Área na Axial responsável pela análise contínua de atendimento as normas, leis e regulamentações destinadas as atividades finais da empresa.</t>
   </si>
   <si>
-    <t>03-Orçamento</t>
+    <t>Orçamento</t>
   </si>
   <si>
     <t>Área da Axial responsável pelas contatos de negociações junto aos clientes da empresa(hospitais, convênios)</t>
   </si>
   <si>
-    <t>04-Comercial</t>
+    <t>Comercial</t>
   </si>
   <si>
     <t>Área da Axial responsável pelo acompanhemento e mantimento de relações externas da empresa, estreitando relações com entidades do segmento. Acompanhamento de procedimentos e pendências de faturamento externas.</t>
   </si>
   <si>
-    <t>05-Instrumentação</t>
+    <t>Instrumentação</t>
   </si>
   <si>
     <t>Área da Axial responsável pelos ativos em um procedimento atendido pela empresa.</t>
   </si>
   <si>
-    <t>06-Fiscal</t>
-  </si>
-  <si>
-    <t>07-Estoque</t>
-  </si>
-  <si>
-    <t>08-Compras</t>
-  </si>
-  <si>
-    <t>09-Acopanhamento Axial</t>
-  </si>
-  <si>
-    <t>Área inexistente de apoio da equipe de qualidade a todos os processos da Axial. (remo)</t>
-  </si>
-  <si>
-    <t>10-Cadastro de produto</t>
+    <t>Fiscal</t>
+  </si>
+  <si>
+    <t>Estoque</t>
+  </si>
+  <si>
+    <t>Compras</t>
+  </si>
+  <si>
+    <t>Mantimento de produto</t>
   </si>
   <si>
     <t>Área na Axial responsável pelo tramite de um produto dentro do contexto da Axial, com as variações (material., equipamento e sub).</t>
   </si>
   <si>
+    <t>Distribuição</t>
+  </si>
+  <si>
     <t>Atividade de Negócio</t>
   </si>
   <si>
     <t xml:space="preserve">1. Atividades de negócio (ATN), são realizadas por uma área. É possível que uma atividade seja executada por mais de uma área de negócio.
+2. Uma ATN pode ser equivalente a um processo de negócio sob a ótica da BPMN.
 </t>
   </si>
   <si>
     <t>Descrição da Atividade de negócio</t>
   </si>
   <si>
-    <t>01-Análise regulatória do fornecedor</t>
+    <t>Análise regulatória do fornecedor</t>
   </si>
   <si>
     <t>Atividade onde a equipe analisa se o fornecedor está aderente as regulamentações aplicáveis. Esta atividade é essencial para a garantia de parceria regular com o fornecedor. Neste  momento os fornecedores são subdivididos em 3 grupos (aprovados, em análise e reprovados) que dará subsídio para análise regulatória, podendo o fornecedor ter as relações comerciais suspensas enquanto a regularização não ocorre. Nesta atividade inclusive, existem gatilhos para outros processos como: Análise fiscal (feito pelo financeiro)</t>
   </si>
   <si>
-    <t>02-Análise fiscal do fornecedor</t>
+    <t>Análise fiscal do fornecedor</t>
   </si>
   <si>
     <t>***DEFINIR COM EQUIPE FINANCEIRA (acreditoq eu conjunto de responsabilidades fiscais obrigatórias (feat. SEFAZ, GFIP, SOF, ETC)</t>
   </si>
   <si>
-    <t>03-Inspesão</t>
-  </si>
-  <si>
-    <t>Atividade de negócio onde a equipe realiza inspesão visual no material recebido, conferência (recebimento de logistica-batimento) com a nota fiscal, gera o registro de inspesão (onde é definido se o produto é conforme ou não-conforme).</t>
-  </si>
-  <si>
-    <t>03-Axial/Logística/Estoque</t>
-  </si>
-  <si>
-    <t>04-Recebimento de materiais</t>
+    <t>Inspeção</t>
+  </si>
+  <si>
+    <t>Atividade de negócio onde a equipe realiza inspesão visual no material recebido, conferência (recebimento de logistica-batimento) com a nota fiscal, gera o registro de inspeção (onde é definido se o produto é conforme ou não-conforme).</t>
+  </si>
+  <si>
+    <t>Recebimento de materiais</t>
   </si>
   <si>
     <t>Equipe de estoque realiza a entrada dos itens da nota no estoque, gera o e-lote(rastreabilidade), embala o produto e cataloga com as etiquetas de identificação adequadas (Verde, Amarela e Vermelha). A equipe gera a planilha de rastreabilidade de itens da entrada e encaminha para os envolvidos.</t>
   </si>
   <si>
-    <t>05-Apuração de falha</t>
+    <t>Apuração de falha</t>
   </si>
   <si>
     <t>Gerado por uma não-conformidade de utilização, é na apuração onde se detecta (no ato cirúrgico, em estoque interno, distribuído ou qualquer outro contexto onde um ativo da Axial seja protagonista de uma não-conformidade) um erro de fabricação, uma má conduta médica, contaminação, uma falha na estrutura física e climática do hospital.</t>
   </si>
   <si>
-    <t>06-Auditoria de qualidade do estoque local</t>
-  </si>
-  <si>
-    <t>(SERÁ SUB DE AUDITORIA)</t>
-  </si>
-  <si>
-    <t>07-Auditoria de qualidade do estoque distribuído</t>
-  </si>
-  <si>
-    <t>08-Análise de lições aprendidas</t>
+    <t>Análise de lições aprendidas</t>
   </si>
   <si>
     <t xml:space="preserve">Análise realizada pela equipe de auditoria da qualidade em consequência de um evento para enfatizar as ocorrências positivas e negativas, propondo continuidade dos ganhos e definindo ações de atuação nas falhas. 
 O final de uma análise é marcado pela realização de feedback(reunião geral, ou direcionada, seguida de possíveis ações de treinamento, capacitação e etc) da análise para os demais colaboradores da empresa. </t>
   </si>
   <si>
-    <t>09-Auditoria de qualidade</t>
+    <t>Auditoria de qualidade</t>
   </si>
   <si>
     <t>Realizada anualmente tem como objetivo gerar gatilhos de atividades acerca das diretrizes de qualidade adotadas pela Axial, desde a inspesão física climática, ambiental, sanitária e inspesão regulatória de fornecedores. Como atualização de rastreabilidade de ativos da empresa. Acompanhamento de satisfação e relacionamento com fornecedores e clientes. Análise de conformidade(estado, validade, posição de estoque, etc) dos produtos consignados nos estoque distribuídos da Axial(hospitais e outros) e estoque local. Necessariamente deve acontecer uma análise de lições aprendidas(SERÀ UM MACRO)</t>
   </si>
   <si>
-    <t>10-Iniciar pedido de compra</t>
+    <t>Iniciar pedido de compra</t>
   </si>
   <si>
     <t xml:space="preserve">É dado inicio no processo de pedido de compra, onde as áreas responsáveis </t>
   </si>
   <si>
-    <t>11-Cadastro de produtos</t>
+    <t>Cadastro de produtos</t>
+  </si>
+  <si>
+    <t>Atividade de cadastro de produtos trabalhlados pela empresa no sistema de gestão, considerando sua tabela de preços e contratos com fornecedores, é nessa atividade também que são montados os kits cirúrgicos.</t>
   </si>
   <si>
     <t>Ação do Fluxo de Negócio</t>
@@ -265,7 +252,7 @@
     <t>...na ação</t>
   </si>
   <si>
-    <t>01-Levantar regulamentação necessária</t>
+    <t>Levantar regulamentação necessária</t>
   </si>
   <si>
     <t>Caso o fornecedor, seja elegível a avaliação regulatória da RCD16-2013 ou equivalente(de acordo com o segmento do fornecedor) a equipe levanta quais exigências de regulamentação são elegíveis ao contexto do fornecedor para um determinado material. Estas exigências são analisadas pela equipe responsável na Axial, em seguida repassada para validação do fornecedor.</t>
@@ -274,7 +261,7 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>02-Enviar exigências ao fornecedor</t>
+    <t>Enviar exigências ao fornecedor</t>
   </si>
   <si>
     <t>As regulamentações levantadas pela equipe da Axial é enviada para o fornecedor pelos meios disponíveis, as exigências são enviadas com os devidos embasamentos. A equipe deve monitorar para que o fornecedor forneça um retorno em tempo hábil ao prazo máximo de aquisição.
@@ -287,7 +274,7 @@
     <t>o material do fornecedor em questão seja elegível</t>
   </si>
   <si>
-    <t>03-Analisar feedback do fornecedor</t>
+    <t>Analisar feedback do fornecedor</t>
   </si>
   <si>
     <t>Equipe recebe, analisa e atualiza no sistema a documentação enviada pelo fornecedor.
@@ -299,7 +286,7 @@
     <t>o fornecedor analisar e retornar</t>
   </si>
   <si>
-    <t>04-Enviar documentação regulatória ao fornecedor</t>
+    <t>Enviar documentação regulatória ao fornecedor</t>
   </si>
   <si>
     <t>Equipe responsável na Axial, prepara e envia documentação regulatória ao fornecedor. (contrato social, AFE (autorização de funcionamento especial), licença de funcionamento, licença de vigilância sanitária, etc)
@@ -309,7 +296,7 @@
     <t>o fornecedor solicitar documentação</t>
   </si>
   <si>
-    <t>05-Receber contrato do fornecedor</t>
+    <t>Receber contrato do fornecedor</t>
   </si>
   <si>
     <t>Equipe de qualidade, recebe a analisa o contrato enviado pelo fornecedor, com a perspectiva de acompanhamento dos materiais e condições de relacionamento baseado nas normativas e etc.
@@ -319,19 +306,19 @@
     <t>o fornecedor enviar o contrato</t>
   </si>
   <si>
-    <t>06-Coletar tabela de preços</t>
+    <t>Coletar tabela de preços</t>
   </si>
   <si>
     <t>Equipe coleta do fornecedor a tabela de preços praticados para um determnado produto, para que seja utilizado como base de valores de um produto caadstrado no sistema.</t>
   </si>
   <si>
-    <t>07-Avaliação Jurídica do contrato</t>
+    <t>Avaliação Jurídica do contrato</t>
   </si>
   <si>
     <t>Equipe externa que avalia as codições jurídicas do contrato e atesta a validade.</t>
   </si>
   <si>
-    <t>07-Incluir o produto no sistema</t>
+    <t>Incluir produto no sistema</t>
   </si>
   <si>
     <t>Cadastra as informações básicas de um produto:
@@ -342,13 +329,13 @@
 - registro anvisa, classificação de risco, validade ou vigência do produto na Anvisa (**possibilitar integração com REST API da ANVISA, a necessidade é recorrente e pode gerar dados inconsistentes).</t>
   </si>
   <si>
-    <t>08-Criar Kit  Cirúrgico</t>
+    <t>Criar Kit  Cirúrgico</t>
   </si>
   <si>
     <t>Equipe monta um novo kit cirúrgico com os devidos produtos e quantidades. (Tratar kit com herança dos produtos de sua composição, inclusive validade/vigência, fabricante, divisão, linha, modelo, referência e etc.)</t>
   </si>
   <si>
-    <t>09-Criar Contrato</t>
+    <t>Criar Contrato</t>
   </si>
   <si>
     <t>Equipe cria um objeto de contrato dentro do sistema, para estabelecer as diretrizes básicas entre um fornecedor com um determinado produto/conjunto de produtos e as expectativas da Axial enquanto consumidor intermediario.
@@ -365,16 +352,17 @@
   <si>
     <t>1. Expectativas (EXP), são definidas com base na relação das atividades de negócio da área que serão executadas com apoio da solução.
 2. São essenciais para a clareza de reais problemas de negócio.
-3. Após o claro entendimento das expectativas da área com relação a solução, a definição de um problema tende à ser mais fluída.</t>
+3. Após o claro entendimento das expectativas da área com relação a solução, a definição de um problema tende à ser mais fluída.
+4. As expectativas tornam-se naturalmente critérios de aceite de uma solução para uma determinada área de negócio.</t>
   </si>
   <si>
     <t>Expectativa</t>
   </si>
   <si>
-    <t>01-Que todo fornecedor da Axial possa ser submetido a uma verificação regulatória</t>
-  </si>
-  <si>
-    <t>02-Que as regulamentações externas acerca de um material sejam atendidas</t>
+    <t>Que todo fornecedor da Axial possa ser submetido a uma verificação regulatória</t>
+  </si>
+  <si>
+    <t>Que as regulamentações externas acerca de um material sejam atendidas</t>
   </si>
   <si>
     <t>Problematização</t>
@@ -519,11 +507,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -549,11 +537,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -564,11 +574,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -581,15 +598,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -605,14 +623,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -620,7 +645,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -641,28 +666,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -671,23 +674,15 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -715,13 +710,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -739,43 +818,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -787,13 +836,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -805,7 +848,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -823,37 +866,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -865,37 +884,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -998,26 +993,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1038,16 +1033,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1059,15 +1054,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1086,155 +1072,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1265,6 +1260,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1291,6 +1289,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1649,88 +1648,88 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A24" sqref="A23:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="27.8583333333333" customWidth="1"/>
+    <col min="1" max="1" width="39.625" customWidth="1"/>
     <col min="2" max="2" width="17.2833333333333" customWidth="1"/>
     <col min="3" max="3" width="58.2833333333333" customWidth="1"/>
     <col min="4" max="4" width="32.2833333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" spans="1:7">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-    </row>
-    <row r="2" s="18" customFormat="1" spans="1:7">
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+    </row>
+    <row r="2" s="19" customFormat="1" spans="1:7">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-    </row>
-    <row r="3" s="18" customFormat="1" spans="1:7">
+      <c r="D2" s="13"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+    </row>
+    <row r="3" s="19" customFormat="1" spans="1:7">
       <c r="A3" s="6"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-    </row>
-    <row r="4" s="18" customFormat="1" spans="1:7">
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+    </row>
+    <row r="4" s="19" customFormat="1" spans="1:7">
       <c r="A4" s="6"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-    </row>
-    <row r="5" s="18" customFormat="1" spans="1:7">
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+    </row>
+    <row r="5" s="19" customFormat="1" spans="1:7">
       <c r="A5" s="6"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-    </row>
-    <row r="6" s="18" customFormat="1" spans="1:7">
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+    </row>
+    <row r="6" s="19" customFormat="1" spans="1:7">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="5:7">
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="23" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="23" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1744,7 +1743,7 @@
       <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="19" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1752,30 +1751,33 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="C10" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>12</v>
+      <c r="A11" s="25" t="s">
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>15</v>
+      <c r="A12" s="25" t="s">
+        <v>13</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -1788,28 +1790,28 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" t="s">
+      <c r="A13" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" t="s">
+      <c r="A14" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
         <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>
@@ -1817,13 +1819,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
         <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
@@ -1842,146 +1844,146 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G117"/>
+  <dimension ref="A1:G116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="27.8583333333333" customWidth="1"/>
-    <col min="2" max="2" width="23.125" customWidth="1"/>
+    <col min="1" max="1" width="29.625" customWidth="1"/>
+    <col min="2" max="2" width="21.125" customWidth="1"/>
     <col min="3" max="3" width="70.5666666666667" customWidth="1"/>
     <col min="4" max="4" width="9.14166666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" spans="1:1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" s="19" customFormat="1" spans="1:7">
+      <c r="A2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="36"/>
+    </row>
+    <row r="3" s="19" customFormat="1" spans="1:7">
+      <c r="A3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="37"/>
+    </row>
+    <row r="4" s="19" customFormat="1" spans="1:7">
+      <c r="A4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="37"/>
+    </row>
+    <row r="5" s="19" customFormat="1" spans="1:7">
+      <c r="A5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="37"/>
+    </row>
+    <row r="6" s="19" customFormat="1" spans="1:7">
+      <c r="A6" s="33"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="38"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="23" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" s="18" customFormat="1" spans="1:7">
-      <c r="A2" s="4" t="s">
+      <c r="C8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="34"/>
-    </row>
-    <row r="3" s="18" customFormat="1" spans="1:7">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="35"/>
-    </row>
-    <row r="4" s="18" customFormat="1" spans="1:7">
-      <c r="A4" s="29"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="35"/>
-    </row>
-    <row r="5" s="18" customFormat="1" spans="1:7">
-      <c r="A5" s="29"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="35"/>
-    </row>
-    <row r="6" s="18" customFormat="1" spans="1:7">
-      <c r="A6" s="31"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="36"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="23"/>
+      <c r="D8" s="24"/>
     </row>
     <row r="9" ht="25.5" spans="1:4">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="19"/>
+    </row>
+    <row r="10" ht="25.5" spans="1:3">
+      <c r="A10" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D9" s="18"/>
-    </row>
-    <row r="10" ht="25.5" spans="1:3">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="11" ht="25.5" spans="1:3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" ht="38.25" spans="1:3">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="14" spans="1:3">
+      <c r="A14" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>39</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
       </c>
       <c r="C14" s="2"/>
     </row>
@@ -1990,40 +1992,38 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" ht="25.5" spans="1:3">
+      <c r="A17" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" ht="25.5" spans="1:3">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" ht="25.5" spans="1:3">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="C18" s="2"/>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" s="2"/>
@@ -2318,16 +2318,13 @@
     </row>
     <row r="116" spans="3:3">
       <c r="C116" s="2"/>
-    </row>
-    <row r="117" spans="3:3">
-      <c r="C117" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:G6"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A18;A9:A17;A19:A109">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9;A10;A13;A14;A15;A16;A11:A12;A17:A18;A19:A108">
       <formula1>PI!$A$9:$A$109</formula1>
     </dataValidation>
   </dataValidations>
@@ -2339,527 +2336,580 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G118"/>
+  <dimension ref="A1:G174"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="27.8583333333333" customWidth="1"/>
-    <col min="2" max="2" width="21.875" customWidth="1"/>
-    <col min="3" max="3" width="43.125" customWidth="1"/>
+    <col min="1" max="1" width="28.875" customWidth="1"/>
+    <col min="2" max="2" width="33.125" customWidth="1"/>
+    <col min="3" max="3" width="62.875" customWidth="1"/>
     <col min="4" max="4" width="58.5666666666667" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" spans="1:1">
-      <c r="A1" s="19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" s="18" customFormat="1" spans="1:7">
+      <c r="A1" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" s="19" customFormat="1" spans="1:7">
       <c r="A2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
+        <v>46</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="34"/>
-    </row>
-    <row r="3" s="18" customFormat="1" spans="1:7">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="36"/>
+    </row>
+    <row r="3" s="19" customFormat="1" spans="1:7">
+      <c r="A3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="35"/>
-    </row>
-    <row r="4" s="18" customFormat="1" spans="1:7">
-      <c r="A4" s="29"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="37"/>
+    </row>
+    <row r="4" s="19" customFormat="1" spans="1:7">
+      <c r="A4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="7"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="35"/>
-    </row>
-    <row r="5" s="18" customFormat="1" spans="1:7">
-      <c r="A5" s="29"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="37"/>
+    </row>
+    <row r="5" s="19" customFormat="1" spans="1:7">
+      <c r="A5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="35"/>
-    </row>
-    <row r="6" s="18" customFormat="1" spans="1:7">
-      <c r="A6" s="31"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="37"/>
+    </row>
+    <row r="6" s="19" customFormat="1" spans="1:7">
+      <c r="A6" s="33"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="36"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="22" t="str">
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="38"/>
+    </row>
+    <row r="7" spans="3:3">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="23" t="str">
         <f>"AN"</f>
         <v>AN</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="B8" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" ht="102" spans="1:3">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="C9" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" ht="25.5" spans="1:3">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" ht="102" spans="1:4">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="C10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="2" t="s">
+    </row>
+    <row r="11" ht="51" spans="1:3">
+      <c r="A11" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="10" ht="25.5" spans="1:4">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C11" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" ht="63.75" spans="1:3">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" ht="63.75" spans="1:3">
+      <c r="A13" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" ht="89.25" spans="1:3">
+      <c r="A14" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" ht="114.75" spans="1:3">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" ht="25.5" spans="1:3">
+      <c r="A16" t="s">
         <v>41</v>
       </c>
-      <c r="C10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" ht="51" spans="1:4">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" ht="63.75" spans="1:4">
-      <c r="A12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="B16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" ht="38.25" spans="1:3">
+      <c r="A17" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" ht="76.5" spans="1:4">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="33" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" ht="114.75" spans="1:4">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" ht="127.5" spans="1:4">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" ht="25.5" spans="1:4">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3">
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="3:3">
+    <row r="21" spans="2:3">
+      <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="3:3">
+    <row r="22" spans="2:3">
+      <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="3:3">
+    <row r="23" spans="2:3">
+      <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="3:3">
+    <row r="24" spans="2:3">
+      <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="3:3">
+    <row r="25" spans="2:3">
+      <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="3:3">
+    <row r="26" spans="2:3">
+      <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="3:3">
+    <row r="27" spans="2:3">
+      <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="3:3">
+    <row r="28" spans="2:3">
+      <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="3:3">
+    <row r="29" spans="2:3">
+      <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="3:3">
+    <row r="30" spans="2:3">
+      <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="3:3">
+    <row r="31" spans="2:3">
+      <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="3:3">
+    <row r="32" spans="2:3">
+      <c r="B32" s="2"/>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="3:3">
+    <row r="33" spans="2:3">
+      <c r="B33" s="2"/>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="3:3">
+    <row r="34" spans="2:3">
+      <c r="B34" s="2"/>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="3:3">
+    <row r="35" spans="2:3">
+      <c r="B35" s="2"/>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="3:3">
+    <row r="36" spans="2:3">
+      <c r="B36" s="2"/>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="3:3">
+    <row r="37" spans="2:3">
+      <c r="B37" s="2"/>
       <c r="C37" s="2"/>
     </row>
-    <row r="38" spans="3:3">
+    <row r="38" spans="2:3">
+      <c r="B38" s="2"/>
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="3:3">
+    <row r="39" spans="2:3">
+      <c r="B39" s="2"/>
       <c r="C39" s="2"/>
     </row>
-    <row r="40" spans="3:3">
+    <row r="40" spans="2:3">
+      <c r="B40" s="2"/>
       <c r="C40" s="2"/>
     </row>
-    <row r="41" spans="3:3">
+    <row r="41" spans="2:3">
+      <c r="B41" s="2"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="3:3">
+    <row r="42" spans="2:3">
+      <c r="B42" s="2"/>
       <c r="C42" s="2"/>
     </row>
-    <row r="43" spans="3:3">
+    <row r="43" spans="2:3">
+      <c r="B43" s="2"/>
       <c r="C43" s="2"/>
     </row>
-    <row r="44" spans="3:3">
+    <row r="44" spans="2:3">
+      <c r="B44" s="2"/>
       <c r="C44" s="2"/>
     </row>
-    <row r="45" spans="3:3">
+    <row r="45" spans="2:3">
+      <c r="B45" s="2"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="3:3">
+    <row r="46" spans="2:3">
+      <c r="B46" s="2"/>
       <c r="C46" s="2"/>
     </row>
-    <row r="47" spans="3:3">
+    <row r="47" spans="2:3">
+      <c r="B47" s="2"/>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="3:3">
+    <row r="48" spans="2:3">
+      <c r="B48" s="2"/>
       <c r="C48" s="2"/>
     </row>
-    <row r="49" spans="3:3">
+    <row r="49" spans="2:3">
+      <c r="B49" s="2"/>
       <c r="C49" s="2"/>
     </row>
-    <row r="50" spans="3:3">
+    <row r="50" spans="2:3">
+      <c r="B50" s="2"/>
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="3:3">
+    <row r="51" spans="2:3">
+      <c r="B51" s="2"/>
       <c r="C51" s="2"/>
     </row>
-    <row r="52" spans="3:3">
+    <row r="52" spans="2:3">
+      <c r="B52" s="2"/>
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="3:3">
+    <row r="53" spans="2:3">
+      <c r="B53" s="2"/>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="3:3">
+    <row r="54" spans="2:3">
+      <c r="B54" s="2"/>
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="3:3">
+    <row r="55" spans="2:3">
+      <c r="B55" s="2"/>
       <c r="C55" s="2"/>
     </row>
-    <row r="56" spans="3:3">
+    <row r="56" spans="2:3">
+      <c r="B56" s="2"/>
       <c r="C56" s="2"/>
     </row>
-    <row r="57" spans="3:3">
+    <row r="57" spans="2:3">
+      <c r="B57" s="2"/>
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="3:3">
+    <row r="58" spans="2:3">
+      <c r="B58" s="2"/>
       <c r="C58" s="2"/>
     </row>
-    <row r="59" spans="3:3">
+    <row r="59" spans="2:3">
+      <c r="B59" s="2"/>
       <c r="C59" s="2"/>
     </row>
-    <row r="60" spans="3:3">
+    <row r="60" spans="2:3">
+      <c r="B60" s="2"/>
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="3:3">
+    <row r="61" spans="2:3">
+      <c r="B61" s="2"/>
       <c r="C61" s="2"/>
     </row>
-    <row r="62" spans="3:3">
+    <row r="62" spans="2:3">
+      <c r="B62" s="2"/>
       <c r="C62" s="2"/>
     </row>
-    <row r="63" spans="3:3">
+    <row r="63" spans="2:3">
+      <c r="B63" s="2"/>
       <c r="C63" s="2"/>
     </row>
-    <row r="64" spans="3:3">
+    <row r="64" spans="2:3">
+      <c r="B64" s="2"/>
       <c r="C64" s="2"/>
     </row>
-    <row r="65" spans="3:3">
+    <row r="65" spans="2:3">
+      <c r="B65" s="2"/>
       <c r="C65" s="2"/>
     </row>
-    <row r="66" spans="3:3">
+    <row r="66" spans="2:3">
+      <c r="B66" s="2"/>
       <c r="C66" s="2"/>
     </row>
-    <row r="67" spans="3:3">
+    <row r="67" spans="2:3">
+      <c r="B67" s="2"/>
       <c r="C67" s="2"/>
     </row>
-    <row r="68" spans="3:3">
+    <row r="68" spans="2:3">
+      <c r="B68" s="2"/>
       <c r="C68" s="2"/>
     </row>
-    <row r="69" spans="3:3">
+    <row r="69" spans="2:3">
+      <c r="B69" s="2"/>
       <c r="C69" s="2"/>
     </row>
-    <row r="70" spans="3:3">
+    <row r="70" spans="2:3">
+      <c r="B70" s="2"/>
       <c r="C70" s="2"/>
     </row>
-    <row r="71" spans="3:3">
+    <row r="71" spans="2:3">
+      <c r="B71" s="2"/>
       <c r="C71" s="2"/>
     </row>
-    <row r="72" spans="3:3">
+    <row r="72" spans="2:3">
+      <c r="B72" s="2"/>
       <c r="C72" s="2"/>
     </row>
-    <row r="73" spans="3:3">
+    <row r="73" spans="2:3">
+      <c r="B73" s="2"/>
       <c r="C73" s="2"/>
     </row>
-    <row r="74" spans="3:3">
+    <row r="74" spans="2:3">
+      <c r="B74" s="2"/>
       <c r="C74" s="2"/>
     </row>
-    <row r="75" spans="3:3">
+    <row r="75" spans="2:3">
+      <c r="B75" s="2"/>
       <c r="C75" s="2"/>
     </row>
-    <row r="76" spans="3:3">
+    <row r="76" spans="2:3">
+      <c r="B76" s="2"/>
       <c r="C76" s="2"/>
     </row>
-    <row r="77" spans="3:3">
+    <row r="77" spans="2:3">
+      <c r="B77" s="2"/>
       <c r="C77" s="2"/>
     </row>
-    <row r="78" spans="3:3">
+    <row r="78" spans="2:3">
+      <c r="B78" s="2"/>
       <c r="C78" s="2"/>
     </row>
-    <row r="79" spans="3:3">
+    <row r="79" spans="2:3">
+      <c r="B79" s="2"/>
       <c r="C79" s="2"/>
     </row>
-    <row r="80" spans="3:3">
+    <row r="80" spans="2:3">
+      <c r="B80" s="2"/>
       <c r="C80" s="2"/>
     </row>
-    <row r="81" spans="3:3">
+    <row r="81" spans="2:3">
+      <c r="B81" s="2"/>
       <c r="C81" s="2"/>
     </row>
-    <row r="82" spans="3:3">
+    <row r="82" spans="2:3">
+      <c r="B82" s="2"/>
       <c r="C82" s="2"/>
     </row>
-    <row r="83" spans="3:3">
+    <row r="83" spans="2:3">
+      <c r="B83" s="2"/>
       <c r="C83" s="2"/>
     </row>
-    <row r="84" spans="3:3">
+    <row r="84" spans="2:3">
+      <c r="B84" s="2"/>
       <c r="C84" s="2"/>
     </row>
-    <row r="85" spans="3:3">
+    <row r="85" spans="2:3">
+      <c r="B85" s="2"/>
       <c r="C85" s="2"/>
     </row>
-    <row r="86" spans="3:3">
+    <row r="86" spans="2:3">
+      <c r="B86" s="2"/>
       <c r="C86" s="2"/>
     </row>
-    <row r="87" spans="3:3">
+    <row r="87" spans="2:3">
+      <c r="B87" s="2"/>
       <c r="C87" s="2"/>
     </row>
-    <row r="88" spans="3:3">
+    <row r="88" spans="2:3">
+      <c r="B88" s="2"/>
       <c r="C88" s="2"/>
     </row>
-    <row r="89" spans="3:3">
+    <row r="89" spans="2:3">
+      <c r="B89" s="2"/>
       <c r="C89" s="2"/>
     </row>
-    <row r="90" spans="3:3">
+    <row r="90" spans="2:3">
+      <c r="B90" s="2"/>
       <c r="C90" s="2"/>
     </row>
-    <row r="91" spans="3:3">
+    <row r="91" spans="2:3">
+      <c r="B91" s="2"/>
       <c r="C91" s="2"/>
     </row>
-    <row r="92" spans="3:3">
+    <row r="92" spans="2:3">
+      <c r="B92" s="2"/>
       <c r="C92" s="2"/>
     </row>
-    <row r="93" spans="3:3">
+    <row r="93" spans="2:3">
+      <c r="B93" s="2"/>
       <c r="C93" s="2"/>
     </row>
-    <row r="94" spans="3:3">
+    <row r="94" spans="2:3">
+      <c r="B94" s="2"/>
       <c r="C94" s="2"/>
     </row>
-    <row r="95" spans="3:3">
+    <row r="95" spans="2:3">
+      <c r="B95" s="2"/>
       <c r="C95" s="2"/>
     </row>
-    <row r="96" spans="3:3">
+    <row r="96" spans="2:3">
+      <c r="B96" s="2"/>
       <c r="C96" s="2"/>
     </row>
-    <row r="97" spans="3:3">
+    <row r="97" spans="2:3">
+      <c r="B97" s="2"/>
       <c r="C97" s="2"/>
     </row>
-    <row r="98" spans="3:3">
+    <row r="98" spans="2:3">
+      <c r="B98" s="2"/>
       <c r="C98" s="2"/>
     </row>
-    <row r="99" spans="3:3">
+    <row r="99" spans="2:3">
+      <c r="B99" s="2"/>
       <c r="C99" s="2"/>
     </row>
-    <row r="100" spans="3:3">
+    <row r="100" spans="2:3">
+      <c r="B100" s="2"/>
       <c r="C100" s="2"/>
     </row>
-    <row r="101" spans="3:3">
+    <row r="101" spans="2:3">
+      <c r="B101" s="2"/>
       <c r="C101" s="2"/>
     </row>
-    <row r="102" spans="3:3">
+    <row r="102" spans="2:3">
+      <c r="B102" s="2"/>
       <c r="C102" s="2"/>
     </row>
-    <row r="103" spans="3:3">
+    <row r="103" spans="2:3">
+      <c r="B103" s="2"/>
       <c r="C103" s="2"/>
     </row>
-    <row r="104" spans="3:3">
+    <row r="104" spans="2:3">
+      <c r="B104" s="2"/>
       <c r="C104" s="2"/>
     </row>
-    <row r="105" spans="3:3">
+    <row r="105" spans="2:3">
+      <c r="B105" s="2"/>
       <c r="C105" s="2"/>
     </row>
-    <row r="106" spans="3:3">
+    <row r="106" spans="2:3">
+      <c r="B106" s="2"/>
       <c r="C106" s="2"/>
     </row>
-    <row r="107" spans="3:3">
+    <row r="107" spans="2:3">
+      <c r="B107" s="2"/>
       <c r="C107" s="2"/>
     </row>
-    <row r="108" spans="3:3">
+    <row r="108" spans="2:3">
+      <c r="B108" s="2"/>
       <c r="C108" s="2"/>
     </row>
-    <row r="109" spans="3:3">
+    <row r="109" spans="2:3">
+      <c r="B109" s="2"/>
       <c r="C109" s="2"/>
     </row>
-    <row r="110" spans="3:3">
+    <row r="110" spans="2:3">
+      <c r="B110" s="2"/>
       <c r="C110" s="2"/>
     </row>
-    <row r="111" spans="3:3">
+    <row r="111" spans="2:3">
+      <c r="B111" s="2"/>
       <c r="C111" s="2"/>
     </row>
-    <row r="112" spans="3:3">
+    <row r="112" spans="2:3">
+      <c r="B112" s="2"/>
       <c r="C112" s="2"/>
     </row>
-    <row r="113" spans="3:3">
+    <row r="113" spans="2:3">
+      <c r="B113" s="2"/>
       <c r="C113" s="2"/>
     </row>
-    <row r="114" spans="3:3">
+    <row r="114" spans="2:3">
+      <c r="B114" s="2"/>
       <c r="C114" s="2"/>
     </row>
-    <row r="115" spans="3:3">
+    <row r="115" spans="2:3">
+      <c r="B115" s="2"/>
       <c r="C115" s="2"/>
     </row>
-    <row r="116" spans="3:3">
+    <row r="116" spans="2:3">
+      <c r="B116" s="2"/>
       <c r="C116" s="2"/>
     </row>
     <row r="117" spans="3:3">
@@ -2868,16 +2918,182 @@
     <row r="118" spans="3:3">
       <c r="C118" s="2"/>
     </row>
+    <row r="119" spans="3:3">
+      <c r="C119" s="2"/>
+    </row>
+    <row r="120" spans="3:3">
+      <c r="C120" s="2"/>
+    </row>
+    <row r="121" spans="3:3">
+      <c r="C121" s="2"/>
+    </row>
+    <row r="122" spans="3:3">
+      <c r="C122" s="2"/>
+    </row>
+    <row r="123" spans="3:3">
+      <c r="C123" s="2"/>
+    </row>
+    <row r="124" spans="3:3">
+      <c r="C124" s="2"/>
+    </row>
+    <row r="125" spans="3:3">
+      <c r="C125" s="2"/>
+    </row>
+    <row r="126" spans="3:3">
+      <c r="C126" s="2"/>
+    </row>
+    <row r="127" spans="3:3">
+      <c r="C127" s="2"/>
+    </row>
+    <row r="128" spans="3:3">
+      <c r="C128" s="2"/>
+    </row>
+    <row r="129" spans="3:3">
+      <c r="C129" s="2"/>
+    </row>
+    <row r="130" spans="3:3">
+      <c r="C130" s="2"/>
+    </row>
+    <row r="131" spans="3:3">
+      <c r="C131" s="2"/>
+    </row>
+    <row r="132" spans="3:3">
+      <c r="C132" s="2"/>
+    </row>
+    <row r="133" spans="3:3">
+      <c r="C133" s="2"/>
+    </row>
+    <row r="134" spans="3:3">
+      <c r="C134" s="2"/>
+    </row>
+    <row r="135" spans="3:3">
+      <c r="C135" s="2"/>
+    </row>
+    <row r="136" spans="3:3">
+      <c r="C136" s="2"/>
+    </row>
+    <row r="137" spans="3:3">
+      <c r="C137" s="2"/>
+    </row>
+    <row r="138" spans="3:3">
+      <c r="C138" s="2"/>
+    </row>
+    <row r="139" spans="3:3">
+      <c r="C139" s="2"/>
+    </row>
+    <row r="140" spans="3:3">
+      <c r="C140" s="2"/>
+    </row>
+    <row r="141" spans="3:3">
+      <c r="C141" s="2"/>
+    </row>
+    <row r="142" spans="3:3">
+      <c r="C142" s="2"/>
+    </row>
+    <row r="143" spans="3:3">
+      <c r="C143" s="2"/>
+    </row>
+    <row r="144" spans="3:3">
+      <c r="C144" s="2"/>
+    </row>
+    <row r="145" spans="3:3">
+      <c r="C145" s="2"/>
+    </row>
+    <row r="146" spans="3:3">
+      <c r="C146" s="2"/>
+    </row>
+    <row r="147" spans="3:3">
+      <c r="C147" s="2"/>
+    </row>
+    <row r="148" spans="3:3">
+      <c r="C148" s="2"/>
+    </row>
+    <row r="149" spans="3:3">
+      <c r="C149" s="2"/>
+    </row>
+    <row r="150" spans="3:3">
+      <c r="C150" s="2"/>
+    </row>
+    <row r="151" spans="3:3">
+      <c r="C151" s="2"/>
+    </row>
+    <row r="152" spans="3:3">
+      <c r="C152" s="2"/>
+    </row>
+    <row r="153" spans="3:3">
+      <c r="C153" s="2"/>
+    </row>
+    <row r="154" spans="3:3">
+      <c r="C154" s="2"/>
+    </row>
+    <row r="155" spans="3:3">
+      <c r="C155" s="2"/>
+    </row>
+    <row r="156" spans="3:3">
+      <c r="C156" s="2"/>
+    </row>
+    <row r="157" spans="3:3">
+      <c r="C157" s="2"/>
+    </row>
+    <row r="158" spans="3:3">
+      <c r="C158" s="2"/>
+    </row>
+    <row r="159" spans="3:3">
+      <c r="C159" s="2"/>
+    </row>
+    <row r="160" spans="3:3">
+      <c r="C160" s="2"/>
+    </row>
+    <row r="161" spans="3:3">
+      <c r="C161" s="2"/>
+    </row>
+    <row r="162" spans="3:3">
+      <c r="C162" s="2"/>
+    </row>
+    <row r="163" spans="3:3">
+      <c r="C163" s="2"/>
+    </row>
+    <row r="164" spans="3:3">
+      <c r="C164" s="2"/>
+    </row>
+    <row r="165" spans="3:3">
+      <c r="C165" s="2"/>
+    </row>
+    <row r="166" spans="3:3">
+      <c r="C166" s="2"/>
+    </row>
+    <row r="167" spans="3:3">
+      <c r="C167" s="2"/>
+    </row>
+    <row r="168" spans="3:3">
+      <c r="C168" s="2"/>
+    </row>
+    <row r="169" spans="3:3">
+      <c r="C169" s="2"/>
+    </row>
+    <row r="170" spans="3:3">
+      <c r="C170" s="2"/>
+    </row>
+    <row r="171" spans="3:3">
+      <c r="C171" s="2"/>
+    </row>
+    <row r="172" spans="3:3">
+      <c r="C172" s="2"/>
+    </row>
+    <row r="173" spans="3:3">
+      <c r="C173" s="2"/>
+    </row>
+    <row r="174" spans="3:3">
+      <c r="C174" s="2"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A8:C17"/>
   <mergeCells count="1">
     <mergeCell ref="A2:G6"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12;B17;B9:B11;B13:B16;B18:B110">
-      <formula1>AN!$B$9:$B$109</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A12;A17;A9:A11;A13:A16;A18:A110">
-      <formula1>PI!$A$9:$A$109</formula1>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A11;A12;A13;A14;A15;A9:A10;A16:A108">
+      <formula1>AN!$B$9:$B$108</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
@@ -2891,10 +3107,10 @@
   <sheetPr/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="7"/>
@@ -2910,308 +3126,281 @@
   </cols>
   <sheetData>
     <row r="1" ht="34.5" spans="1:8">
-      <c r="A1" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="A1" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" s="1" customFormat="1" ht="15" customHeight="1" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:8">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:8">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:8">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:8">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
     </row>
     <row r="7" spans="6:8">
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-    </row>
-    <row r="8" ht="25.5" spans="1:8">
-      <c r="A8" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="10" t="str">
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="10" t="str">
         <f>"AN"</f>
         <v>AN</v>
       </c>
+      <c r="B8" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="C8" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="28"/>
+    </row>
+    <row r="9" ht="127.5" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E9" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="10" t="s">
+    </row>
+    <row r="10" ht="306" spans="1:6">
+      <c r="A10" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="D10" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="E10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H8" s="26"/>
-    </row>
-    <row r="9" ht="76.5" spans="1:6">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="F10" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" ht="229.5" spans="1:6">
+      <c r="A11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="10" ht="216.75" spans="1:7">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="F11" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" ht="114.75" spans="1:6">
+      <c r="A12" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" ht="153" spans="1:7">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="F12" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" ht="102" spans="1:6">
+      <c r="A13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" ht="76.5" spans="1:7">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="F13" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" ht="63.75" spans="1:6">
+      <c r="A14" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="E14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" ht="25.5" spans="3:4">
+      <c r="C15" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" ht="63.75" spans="1:7">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E13" s="2" t="s">
+    </row>
+    <row r="16" ht="178.5" spans="1:4">
+      <c r="A16" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" ht="38.25" spans="1:7">
-      <c r="A14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="2" t="s">
+    </row>
+    <row r="17" ht="76.5" spans="1:5">
+      <c r="A17" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" ht="25.5" spans="4:5">
-      <c r="D15" s="2" t="s">
+      <c r="E17" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" ht="318.75" spans="1:4">
+      <c r="A18" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="16" ht="114.75" spans="1:5">
-      <c r="A16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" ht="51" spans="1:6">
-      <c r="A17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" ht="204" spans="1:5">
-      <c r="A18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:E6"/>
   </mergeCells>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12;C13;C14;C15;C18;C9:C11;C16:C17;C19:C68;C69:C110">
-      <formula1>ATVN!$C$9:$C$110</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12;B13;B14;B15;B16;B17;B18;B9:B11;B19:B110">
-      <formula1>AN!$B$9:$B$109</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G14;G9:G13;G15:G110">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G19:G110">
       <formula1>$D$9:$D$110</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A12;A13;A14;A15;A16;A17;A18;A9:A11;A19:A110">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:F61">
+      <formula1>$C$9:$C$48</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A19:A110">
       <formula1>PI!$A$9:$A$109</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12;B13;B14;B15;B16;B17;B18;B9:B11;C19:C68;C69:C110">
+      <formula1>ATVN!$B$9:$B$108</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9;A10;A11;A12;A13;A14;A15;A16;A17;A18;B19:B110">
+      <formula1>AN!$B$9:$B$108</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
@@ -3226,7 +3415,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -3239,20 +3428,20 @@
   </cols>
   <sheetData>
     <row r="1" ht="34.5" spans="1:1">
-      <c r="A1" s="25" t="s">
-        <v>104</v>
+      <c r="A1" s="27" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:7">
       <c r="A2" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="12"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:7">
       <c r="A3" s="6"/>
@@ -3261,7 +3450,7 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="13"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:7">
       <c r="A4" s="6"/>
@@ -3270,7 +3459,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:7">
       <c r="A5" s="6"/>
@@ -3279,7 +3468,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="13"/>
+      <c r="G5" s="14"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:7">
       <c r="A6" s="8"/>
@@ -3288,7 +3477,7 @@
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="14"/>
+      <c r="G6" s="15"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="10" t="s">
@@ -3299,10 +3488,10 @@
         <v>AN</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" ht="25.5" spans="1:4">
@@ -3310,13 +3499,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" ht="25.5" spans="1:4">
@@ -3324,25 +3513,28 @@
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:G6"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C109">
-      <formula1>ATVN!$C$9:$C$110</formula1>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C89">
+      <formula1>ATVN!$B$9:$B$108</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B104">
-      <formula1>AN!$B$9:$B$109</formula1>
+      <formula1>AN!$B$9:$B$108</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C90:C109">
+      <formula1>ATVN!$C$9:$C$108</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A104">
       <formula1>PI!$A$9:$A$109</formula1>
@@ -3360,123 +3552,129 @@
   <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="27.8583333333333" customWidth="1"/>
-    <col min="2" max="2" width="16.5666666666667" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="70.5666666666667" customWidth="1"/>
     <col min="4" max="4" width="9.14166666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" spans="1:8">
-      <c r="A1" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-    </row>
-    <row r="2" s="18" customFormat="1" ht="15" customHeight="1" spans="1:8">
+      <c r="A1" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+    </row>
+    <row r="2" s="19" customFormat="1" ht="15" customHeight="1" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="24"/>
-    </row>
-    <row r="3" s="18" customFormat="1" spans="1:8">
+      <c r="C2" s="13"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="26"/>
+    </row>
+    <row r="3" s="19" customFormat="1" spans="1:8">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="24"/>
-    </row>
-    <row r="4" s="18" customFormat="1" spans="1:8">
+      <c r="C3" s="14"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="26"/>
+    </row>
+    <row r="4" s="19" customFormat="1" spans="1:8">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="24"/>
-    </row>
-    <row r="5" s="18" customFormat="1" spans="1:8">
+      <c r="C4" s="14"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="26"/>
+    </row>
+    <row r="5" s="19" customFormat="1" spans="1:8">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="24"/>
-    </row>
-    <row r="6" s="18" customFormat="1" spans="1:8">
+      <c r="C5" s="14"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="26"/>
+    </row>
+    <row r="6" s="19" customFormat="1" spans="1:8">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="24"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="4:8">
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="22" t="str">
+      <c r="B8" s="23" t="str">
         <f>"AN"</f>
         <v>AN</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
+        <v>105</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="19"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="18"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="3:3">
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="3:3">
@@ -3803,9 +4001,9 @@
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B109">
-      <formula1>AN!$B$9:$B$109</formula1>
+      <formula1>AN!$B$9:$B$108</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A109">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9;A10:A11;A12:A109">
       <formula1>PI!$A$9:$A$109</formula1>
     </dataValidation>
   </dataValidations>
@@ -3819,8 +4017,8 @@
   <sheetPr/>
   <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -3839,21 +4037,21 @@
   <sheetData>
     <row r="1" ht="17.25" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="15" customHeight="1" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="12"/>
-      <c r="I2" s="16" t="s">
-        <v>114</v>
+      <c r="G2" s="13"/>
+      <c r="I2" s="17" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:9">
@@ -3863,9 +4061,9 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="13"/>
-      <c r="I3" s="17" t="s">
-        <v>115</v>
+      <c r="G3" s="14"/>
+      <c r="I3" s="18" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:9">
@@ -3875,9 +4073,9 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="13"/>
-      <c r="I4" s="17" t="s">
-        <v>116</v>
+      <c r="G4" s="14"/>
+      <c r="I4" s="18" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:7">
@@ -3887,7 +4085,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="13"/>
+      <c r="G5" s="14"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:7">
       <c r="A6" s="6"/>
@@ -3896,7 +4094,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="13"/>
+      <c r="G6" s="14"/>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:7">
       <c r="A7" s="6"/>
@@ -3905,7 +4103,7 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="13"/>
+      <c r="G7" s="14"/>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:7">
       <c r="A8" s="6"/>
@@ -3914,7 +4112,7 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="13"/>
+      <c r="G8" s="14"/>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:7">
       <c r="A9" s="8"/>
@@ -3923,7 +4121,7 @@
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="14"/>
+      <c r="G9" s="15"/>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:7">
       <c r="A10" s="7"/>
@@ -3936,117 +4134,117 @@
     </row>
     <row r="11" ht="25.5" spans="1:7">
       <c r="A11" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" ht="25.5" spans="1:7">
+      <c r="A12" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" ht="38.25" spans="1:7">
-      <c r="A12" s="11" t="s">
-        <v>123</v>
-      </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G12" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" ht="25.5" spans="1:7">
+      <c r="A13" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" ht="25.5" spans="1:7">
+      <c r="A14" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" ht="25.5" spans="1:7">
+      <c r="A15" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="13" ht="38.25" spans="1:7">
-      <c r="A13" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" ht="38.25" spans="1:7">
-      <c r="A14" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" ht="38.25" spans="1:7">
-      <c r="A15" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:1">
@@ -4336,23 +4534,23 @@
     <mergeCell ref="A2:G9"/>
   </mergeCells>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12;F13;F14;F15">
-      <formula1>EXPEC!$D$9:$D$100</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12;B13;B14;B15;B16:B112">
-      <formula1>AN!$B$9:$B$109</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12;E13;E14;E15;E16:E109">
-      <formula1>AFN!$D$9:$D$110</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F16:F109">
-      <formula1>ATVN!$C$9:$C$110</formula1>
+      <formula1>ATVN!$C$9:$C$108</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12;D13;D14;D15;D16:D109">
       <formula1>$I$2:$I$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12;C13;C14;C15;A16:A107;C16:C112">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12;E13:E15;E16:E147">
+      <formula1>AFN!$C$9:$C$110</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12;F13:F15">
+      <formula1>EXPEC!$D$9:$D$100</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12;A16:A107;C13:C15;C16:C112">
       <formula1>PI!$A$9:$A$109</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12;B13:B15;B16:B112">
+      <formula1>AN!$B$9:$B$108</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>

</xml_diff>

<commit_message>
inclusão de atividades do fluxo de Entrega de Romaneio
</commit_message>
<xml_diff>
--- a/vbn/cards/Cards_AXIAL-Qualidade.xlsx
+++ b/vbn/cards/Cards_AXIAL-Qualidade.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="8415" activeTab="3"/>
+    <workbookView windowWidth="23400" windowHeight="10950"/>
   </bookViews>
   <sheets>
     <sheet name="PI" sheetId="1" r:id="rId1"/>
@@ -16,14 +16,14 @@
     <sheet name="RS" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ATVN!$A$8:$C$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ATVN!$A$8:$C$19</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181">
   <si>
     <t>Partes Interessadas</t>
   </si>
@@ -66,25 +66,34 @@
     <t>Contribuinte para o tema logistica</t>
   </si>
   <si>
+    <t>Axial/Financeiro (FIN-OR)</t>
+  </si>
+  <si>
+    <t>Dionísio</t>
+  </si>
+  <si>
+    <t>Contribuinte para o tema orçamento</t>
+  </si>
+  <si>
+    <t>Axial/Financeiro (FIN-FA)</t>
+  </si>
+  <si>
+    <t>Rosangela</t>
+  </si>
+  <si>
+    <t>Contribuinte para o tema faturamento</t>
+  </si>
+  <si>
     <t>Axial/Financeiro (FIN)</t>
   </si>
   <si>
-    <t>Dionísio</t>
-  </si>
-  <si>
-    <t>Contribuinte para o tema orçamento</t>
-  </si>
-  <si>
-    <t>Rosangela</t>
-  </si>
-  <si>
-    <t>Contribuinte para o tema faturamento</t>
-  </si>
-  <si>
     <t>Rosalyne</t>
   </si>
   <si>
     <t>Contribuinte para o tema financeiro</t>
+  </si>
+  <si>
+    <t>Axial/Logística (LOG-DIS)</t>
   </si>
   <si>
     <t>Humberto/Tiago</t>
@@ -134,6 +143,9 @@
     <t>Área da Axial responsável pelas contatos de negociações junto aos clientes da empresa(hospitais, convênios)</t>
   </si>
   <si>
+    <t>Faturamento</t>
+  </si>
+  <si>
     <t>Comercial</t>
   </si>
   <si>
@@ -143,7 +155,7 @@
     <t>Instrumentação</t>
   </si>
   <si>
-    <t>Área da Axial responsável pelos ativos em um procedimento atendido pela empresa.</t>
+    <t>Área da Axial responsável pelos ativos em um procedimento atendido pela empresa em cliente. (eventualmente esta área é assumida por representantes comerciais da empresa à depender do contexto)</t>
   </si>
   <si>
     <t>Fiscal</t>
@@ -224,10 +236,28 @@
     <t xml:space="preserve">É dado inicio no processo de pedido de compra, onde as áreas responsáveis </t>
   </si>
   <si>
+    <t>Entrega de romaneio</t>
+  </si>
+  <si>
+    <t>Digitar romaneio</t>
+  </si>
+  <si>
     <t>Cadastro de produtos</t>
   </si>
   <si>
     <t>Atividade de cadastro de produtos trabalhlados pela empresa no sistema de gestão, considerando sua tabela de preços e contratos com fornecedores, é nessa atividade também que são montados os kits cirúrgicos.</t>
+  </si>
+  <si>
+    <t>Abrir procedimento</t>
+  </si>
+  <si>
+    <t>Atividade onde a área comercial, abre um novo procedimento para que as equipes tecnicas envolvidas atuem.</t>
+  </si>
+  <si>
+    <t>Cadastro de proposta comercial</t>
+  </si>
+  <si>
+    <t>Atividade onde a área comercial da Axial, registra uma proposta de atuação para um cliente.</t>
   </si>
   <si>
     <t>Ação do Fluxo de Negócio</t>
@@ -347,6 +377,74 @@
 Possibilitando seleção de acordo com fornecedor e aplicabilidade.</t>
   </si>
   <si>
+    <t>Encerrar procedimento</t>
+  </si>
+  <si>
+    <t>Instrumentador realiza a finalização do procedimento, com a verificação de utilização de produtos.
+- Em caso de NÃO utilização de produtos, a atividade é finalizada sem subsequentes;
+-  Em caso de uso de produtos o fluxo segue.</t>
+  </si>
+  <si>
+    <t>O procedimento médico ter sido finalizado.</t>
+  </si>
+  <si>
+    <t>Preencher romaneio</t>
+  </si>
+  <si>
+    <t>Instrumentador preenche o romaneio com informações do produto utilizado no procedimento.
+- É necessário colar as etiquetas do e-lote no verso do romaneio;
+- É necessário coletar a assinatura do responsável pelo setor no hospital onde o procedimento foi realizado;
+é necessário destacar a segunda via do romaneio e entregar ao cliente.</t>
+  </si>
+  <si>
+    <t>O produto ter sido utilizado no procedimento.</t>
+  </si>
+  <si>
+    <t>Protocolar entrega na Axial</t>
+  </si>
+  <si>
+    <t>Após finalização do procedimento, com ou sem uso de produtos. O instrumentador protocola a entrega de produtos na Axial.
+Em caso de uso de produtos:
+- O romaneio é entregue corretamente preenchido;
+- Os produtos não utilizados são entregos no estoque.
+Em caso de não utilização de produtos:
+- Os produtos são entregues no estoque.</t>
+  </si>
+  <si>
+    <t>Digitar romaneio protocolado</t>
+  </si>
+  <si>
+    <t>Com o romaneio devidamente preenchido e protocolado, a equipe de faturamento coleta do romaneio as informações relevantes para o faturamento do(s) produto(s) utilizado(s) no procedimento.
+- Em seguida a atividade de entrega de romaneio é finalizada.</t>
+  </si>
+  <si>
+    <t>O romaneio ter sido preenchido</t>
+  </si>
+  <si>
+    <t>Abrir proposta comercial</t>
+  </si>
+  <si>
+    <t>Área comercial abre proposta comercial para um determinado cliente da empresa.
+- Deve ser informado o planejamento de procedimentos da proposta;
+- Deve ser informado o valor financiro proposto para cada procedimento</t>
+  </si>
+  <si>
+    <t>Existir captação de novas propostas.</t>
+  </si>
+  <si>
+    <t>Abrir novo procedimento</t>
+  </si>
+  <si>
+    <t>Com a oportunidade de atuação em um determinado procedimento concretizada. A equipe comercial abre um novo procedimento.
+- Deve ser informada a descrição e quantidade de produtos envolvidos no procedimento;
+- É possível sugerir um instrumentador para atuação no procedimento;
+- Deve ser informado o médico do procedimento;
+- Deve ser informado local, data e hora do procedimento.</t>
+  </si>
+  <si>
+    <t>Uma proposta comercial seja concretizada.</t>
+  </si>
+  <si>
     <t>Expectativas da Área de Negócio</t>
   </si>
   <si>
@@ -363,6 +461,27 @@
   </si>
   <si>
     <t>Que as regulamentações externas acerca de um material sejam atendidas</t>
+  </si>
+  <si>
+    <t>Que todo produto utilizado seja obrigatóriamente referenciado em um romaneio.</t>
+  </si>
+  <si>
+    <t>Que seja possível faturar todo produto utilizado por um cliente em procedimento.</t>
+  </si>
+  <si>
+    <t>Que todo romaneio seja devidamente protocolado e autenticado pelos responsáveis no cliente e na Axial com todas as informações necessárias.</t>
+  </si>
+  <si>
+    <t>Que todo produto restante de um procedimento seja devidamente protocolado e entregue de volta no estoque da Axial.</t>
+  </si>
+  <si>
+    <t>Que todo procedimento possa ser finalizado mesmo quando nenhum produto for utilizado.</t>
+  </si>
+  <si>
+    <t>Que toda proposta possa ter os valores calculados automaticamente pelo sistema.</t>
+  </si>
+  <si>
+    <t>Que seja possível abrir um procedimento com as características particulares de cada oportunidade</t>
   </si>
   <si>
     <t>Problematização</t>
@@ -500,16 +619,88 @@
   <si>
     <t>For possível gerar um relatório da análise regulatória de um ou mais fornecedores.</t>
   </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>For possível resgatar no romaneio uma lista de produtos destinados a um determinado procedimento.</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>For possível informar obrigatoriamente os dados do produto utilizado:
+- e-lote;</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>For possível encaminhar versão digital do romaneio para o cliente:
+- permitindo que seja informado e-mail no momento de preenchimento do romaneio.</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>For possível ter a confirmação do instrumentador quanto a lista de produtos devolvidos ao estoque da Axial.</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>For possível ter em um romaneio a autenticação de um colaborador do estoque referente ao recebimento de produtos restantes do procedimento.</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>For possível selecionar um romaneio pré cadastrado e protocolado para inserir informações financeiras para o devido faturamento:
+- informações A;
+- informações B</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>For possível inserir registro fotografico da etiqueta do e-lote do produto anexado ao romaneio em preenchimento.</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>For possível colher a assinatura do responsável pelo setor no cliente e anexar ao romaneio em preenchimento.</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>For possível finalizar um procedimento informando a não utilização de produtos, sem que seja necessáriao o preenchimento de informações referentes ao produto que já faz parte do procedimento aberto.</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>For possível ter calculado o valor de todos os produtos incluidos na proposta comercial.</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>For possível sugerir um instrumentador para um determinado procedimento.
+- O instrumentador pode ser parte da equipe comercial;
+- O instrumentador pode ser parte da equipe de instrumentação.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -544,6 +735,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -555,13 +753,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -589,30 +780,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -621,16 +788,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -653,7 +812,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -666,8 +825,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -681,8 +863,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -701,7 +892,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -710,7 +901,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -722,49 +997,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -776,19 +1021,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -800,55 +1045,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -860,7 +1063,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -872,25 +1075,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1003,6 +1200,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1013,21 +1225,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1049,11 +1246,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1075,161 +1270,163 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1262,7 +1459,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1289,7 +1492,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1318,6 +1520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1326,6 +1529,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1647,8 +1856,8 @@
   <sheetPr/>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A23:A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -1660,76 +1869,76 @@
   </cols>
   <sheetData>
     <row r="1" ht="17.25" spans="1:7">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-    </row>
-    <row r="2" s="19" customFormat="1" spans="1:7">
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+    </row>
+    <row r="2" s="21" customFormat="1" spans="1:7">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-    </row>
-    <row r="3" s="19" customFormat="1" spans="1:7">
+      <c r="D2" s="15"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+    </row>
+    <row r="3" s="21" customFormat="1" spans="1:7">
       <c r="A3" s="6"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-    </row>
-    <row r="4" s="19" customFormat="1" spans="1:7">
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+    </row>
+    <row r="4" s="21" customFormat="1" spans="1:7">
       <c r="A4" s="6"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-    </row>
-    <row r="5" s="19" customFormat="1" spans="1:7">
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+    </row>
+    <row r="5" s="21" customFormat="1" spans="1:7">
       <c r="A5" s="6"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-    </row>
-    <row r="6" s="19" customFormat="1" spans="1:7">
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+    </row>
+    <row r="6" s="21" customFormat="1" spans="1:7">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
     </row>
     <row r="7" spans="5:7">
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="25" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="25" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1743,7 +1952,7 @@
       <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="21" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1751,18 +1960,18 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="21" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="25" t="s">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
@@ -1776,42 +1985,42 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="25" t="s">
-        <v>13</v>
+      <c r="A12" t="s">
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="25" t="s">
-        <v>13</v>
+      <c r="A13" t="s">
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="25" t="s">
-        <v>10</v>
+      <c r="A14" t="s">
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>
@@ -1819,13 +2028,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
@@ -1844,10 +2053,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G116"/>
+  <dimension ref="A1:G117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -1859,90 +2068,90 @@
   </cols>
   <sheetData>
     <row r="1" ht="17.25" spans="1:1">
-      <c r="A1" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" s="19" customFormat="1" spans="1:7">
+      <c r="A1" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" s="21" customFormat="1" spans="1:7">
       <c r="A2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="36"/>
-    </row>
-    <row r="3" s="19" customFormat="1" spans="1:7">
-      <c r="A3" s="31"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="37"/>
-    </row>
-    <row r="4" s="19" customFormat="1" spans="1:7">
-      <c r="A4" s="31"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="37"/>
-    </row>
-    <row r="5" s="19" customFormat="1" spans="1:7">
-      <c r="A5" s="31"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="37"/>
-    </row>
-    <row r="6" s="19" customFormat="1" spans="1:7">
-      <c r="A6" s="33"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="38"/>
+        <v>29</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="38"/>
+    </row>
+    <row r="3" s="21" customFormat="1" spans="1:7">
+      <c r="A3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="39"/>
+    </row>
+    <row r="4" s="21" customFormat="1" spans="1:7">
+      <c r="A4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="39"/>
+    </row>
+    <row r="5" s="21" customFormat="1" spans="1:7">
+      <c r="A5" s="32"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="39"/>
+    </row>
+    <row r="6" s="21" customFormat="1" spans="1:7">
+      <c r="A6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="40"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>27</v>
+      <c r="B8" s="25" t="s">
+        <v>30</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="24"/>
+        <v>31</v>
+      </c>
+      <c r="D8" s="26"/>
     </row>
     <row r="9" ht="25.5" spans="1:4">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="19"/>
+        <v>33</v>
+      </c>
+      <c r="D9" s="21"/>
     </row>
     <row r="10" ht="25.5" spans="1:3">
-      <c r="A10" s="25" t="s">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" ht="25.5" spans="1:3">
@@ -1950,83 +2159,89 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" ht="38.25" spans="1:3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="41"/>
+    </row>
+    <row r="13" ht="38.25" spans="1:3">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" ht="38.25" spans="1:3">
+      <c r="A14" t="s">
         <v>6</v>
       </c>
-      <c r="B13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="25" t="s">
-        <v>13</v>
-      </c>
       <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="42"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="25" t="s">
-        <v>13</v>
-      </c>
       <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" ht="25.5" spans="1:3">
-      <c r="A17" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="42"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="42"/>
+    </row>
+    <row r="18" ht="25.5" spans="1:3">
+      <c r="A18" t="s">
         <v>10</v>
       </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="25" t="s">
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="B18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="3:3">
-      <c r="C19" s="2"/>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="42"/>
     </row>
     <row r="20" spans="3:3">
       <c r="C20" s="2"/>
@@ -2318,13 +2533,16 @@
     </row>
     <row r="116" spans="3:3">
       <c r="C116" s="2"/>
+    </row>
+    <row r="117" spans="3:3">
+      <c r="C117" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:G6"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9;A10;A13;A14;A15;A16;A11:A12;A17:A18;A19:A108">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9;A10;A11;A12;A13;A14;A15;A16;A17;A18:A19;A20:A109">
       <formula1>PI!$A$9:$A$109</formula1>
     </dataValidation>
   </dataValidations>
@@ -2336,10 +2554,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G174"/>
+  <dimension ref="A1:G176"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -2351,186 +2569,210 @@
   </cols>
   <sheetData>
     <row r="1" ht="17.25" spans="1:1">
-      <c r="A1" s="20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" s="19" customFormat="1" spans="1:7">
+      <c r="A1" s="22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" s="21" customFormat="1" spans="1:7">
       <c r="A2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
+        <v>50</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="36"/>
-    </row>
-    <row r="3" s="19" customFormat="1" spans="1:7">
-      <c r="A3" s="31"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="38"/>
+    </row>
+    <row r="3" s="21" customFormat="1" spans="1:7">
+      <c r="A3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="37"/>
-    </row>
-    <row r="4" s="19" customFormat="1" spans="1:7">
-      <c r="A4" s="31"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="39"/>
+    </row>
+    <row r="4" s="21" customFormat="1" spans="1:7">
+      <c r="A4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="7"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="37"/>
-    </row>
-    <row r="5" s="19" customFormat="1" spans="1:7">
-      <c r="A5" s="31"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="39"/>
+    </row>
+    <row r="5" s="21" customFormat="1" spans="1:7">
+      <c r="A5" s="32"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="37"/>
-    </row>
-    <row r="6" s="19" customFormat="1" spans="1:7">
-      <c r="A6" s="33"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="39"/>
+    </row>
+    <row r="6" s="21" customFormat="1" spans="1:7">
+      <c r="A6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="38"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="40"/>
     </row>
     <row r="7" spans="3:3">
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="23" t="str">
+      <c r="A8" s="25" t="str">
         <f>"AN"</f>
         <v>AN</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>45</v>
+      <c r="B8" s="25" t="s">
+        <v>49</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" ht="102" spans="1:3">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" ht="25.5" spans="1:3">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" ht="51" spans="1:3">
-      <c r="A11" s="25" t="s">
-        <v>31</v>
+      <c r="A11" t="s">
+        <v>34</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" ht="63.75" spans="1:3">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" ht="63.75" spans="1:3">
-      <c r="A13" s="25" t="s">
-        <v>31</v>
+      <c r="A13" t="s">
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>57</v>
+        <v>60</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="14" ht="89.25" spans="1:3">
-      <c r="A14" s="25" t="s">
-        <v>29</v>
+      <c r="A14" t="s">
+        <v>32</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" ht="114.75" spans="1:3">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" ht="25.5" spans="1:3">
       <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" ht="38.25" spans="1:3">
-      <c r="A17" t="s">
-        <v>42</v>
-      </c>
       <c r="B17" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="2:3">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="C17" s="13"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="13"/>
+    </row>
+    <row r="19" ht="38.25" spans="1:3">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" ht="25.5" spans="1:3">
+      <c r="A20" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" ht="25.5" spans="1:3">
+      <c r="A21" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="2"/>
@@ -2912,10 +3154,12 @@
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
     </row>
-    <row r="117" spans="3:3">
+    <row r="117" spans="2:3">
+      <c r="B117" s="2"/>
       <c r="C117" s="2"/>
     </row>
-    <row r="118" spans="3:3">
+    <row r="118" spans="2:3">
+      <c r="B118" s="2"/>
       <c r="C118" s="2"/>
     </row>
     <row r="119" spans="3:3">
@@ -3086,14 +3330,20 @@
     <row r="174" spans="3:3">
       <c r="C174" s="2"/>
     </row>
+    <row r="175" spans="3:3">
+      <c r="C175" s="2"/>
+    </row>
+    <row r="176" spans="3:3">
+      <c r="C176" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A8:C17"/>
+  <autoFilter ref="A8:C19"/>
   <mergeCells count="1">
     <mergeCell ref="A2:G6"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A11;A12;A13;A14;A15;A9:A10;A16:A108">
-      <formula1>AN!$B$9:$B$108</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A11;A12;A13;A14;A15;A16;A17;A18;A9:A10;A19:A110">
+      <formula1>AN!$B$9:$B$109</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
@@ -3105,12 +3355,12 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="7"/>
@@ -3126,69 +3376,69 @@
   </cols>
   <sheetData>
     <row r="1" ht="34.5" spans="1:8">
-      <c r="A1" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="A1" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" s="1" customFormat="1" ht="15" customHeight="1" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:8">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:8">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:8">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:8">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
     </row>
     <row r="7" spans="6:8">
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="10" t="str">
@@ -3196,211 +3446,328 @@
         <v>AN</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="H8" s="28"/>
+        <v>82</v>
+      </c>
+      <c r="H8" s="29"/>
     </row>
     <row r="9" ht="127.5" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" ht="306" spans="1:6">
-      <c r="A10" s="12" t="s">
-        <v>31</v>
+      <c r="A10" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" ht="229.5" spans="1:6">
-      <c r="A11" s="12" t="s">
-        <v>31</v>
+      <c r="A11" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" ht="114.75" spans="1:6">
-      <c r="A12" s="12" t="s">
-        <v>31</v>
+      <c r="A12" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="13" ht="102" spans="1:6">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="14" ht="63.75" spans="1:6">
-      <c r="A14" s="12" t="s">
-        <v>42</v>
+      <c r="A14" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" ht="25.5" spans="3:4">
       <c r="C15" s="2" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" ht="178.5" spans="1:4">
-      <c r="A16" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>64</v>
+      <c r="A16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" ht="76.5" spans="1:5">
-      <c r="A17" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>64</v>
+      <c r="A17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" ht="318.75" spans="1:4">
-      <c r="A18" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>64</v>
+      <c r="A18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>97</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" ht="102" spans="1:6">
+      <c r="A19" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" ht="140.25" spans="1:6">
+      <c r="A20" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" ht="153" spans="1:6">
+      <c r="A21" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" ht="102" spans="1:6">
+      <c r="A22" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" ht="89.25" spans="1:6">
+      <c r="A23" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F23" s="13"/>
+    </row>
+    <row r="24" ht="178.5" spans="1:6">
+      <c r="A24" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:E6"/>
   </mergeCells>
-  <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G19:G110">
-      <formula1>$D$9:$D$110</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:F61">
-      <formula1>$C$9:$C$48</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A19:A110">
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A66:A111">
       <formula1>PI!$A$9:$A$109</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12;B13;B14;B15;B16;B17;B18;B9:B11;C19:C68;C69:C110">
-      <formula1>ATVN!$B$9:$B$108</formula1>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C23;C19:C22;C24:C1048576"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G23;G19:G22;G24:G111">
+      <formula1>$D$9:$D$111</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9;A10;A11;A12;A13;A14;A15;A16;A17;A18;B19:B110">
-      <formula1>AN!$B$9:$B$108</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F23;F9:F22;F24:F62">
+      <formula1>$C$9:$C$49</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12;B13;B14;B15;B16;B17;B23;B9:B11;B18:B22;B24:B76">
+      <formula1>ATVN!$B$9:$B$110</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9;A10;A11;A12;A13;A14;A15;A16;A17;A23;A18:A22;A24:A65;B77:B111">
+      <formula1>AN!$B$9:$B$109</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
@@ -3412,10 +3779,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A17" sqref="A17:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -3428,20 +3795,20 @@
   </cols>
   <sheetData>
     <row r="1" ht="34.5" spans="1:1">
-      <c r="A1" s="27" t="s">
-        <v>98</v>
+      <c r="A1" s="28" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:7">
       <c r="A2" s="4" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="13"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:7">
       <c r="A3" s="6"/>
@@ -3450,7 +3817,7 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="14"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:7">
       <c r="A4" s="6"/>
@@ -3459,7 +3826,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="14"/>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:7">
       <c r="A5" s="6"/>
@@ -3468,7 +3835,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="14"/>
+      <c r="G5" s="16"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:7">
       <c r="A6" s="8"/>
@@ -3477,7 +3844,7 @@
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="15"/>
+      <c r="G6" s="17"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="10" t="s">
@@ -3488,10 +3855,10 @@
         <v>AN</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" ht="25.5" spans="1:4">
@@ -3499,13 +3866,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" ht="25.5" spans="1:4">
@@ -3513,13 +3880,111 @@
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>102</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" ht="25.5" spans="1:4">
+      <c r="A11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" ht="25.5" spans="1:4">
+      <c r="A12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" ht="38.25" spans="1:4">
+      <c r="A13" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" ht="25.5" spans="1:4">
+      <c r="A14" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" ht="25.5" spans="1:4">
+      <c r="A15" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" ht="25.5" spans="1:4">
+      <c r="A16" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" ht="25.5" spans="1:4">
+      <c r="A17" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -3527,16 +3992,16 @@
     <mergeCell ref="A2:G6"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C89">
-      <formula1>ATVN!$B$9:$B$108</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C91:C110">
+      <formula1>ATVN!$C$9:$C$110</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B104">
-      <formula1>AN!$B$9:$B$108</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12;C15;C9:C11;C13:C14;C16:C90">
+      <formula1>ATVN!$B$9:$B$110</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C90:C109">
-      <formula1>ATVN!$C$9:$C$108</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12;B15;B9:B11;B13:B14;B16:B105">
+      <formula1>AN!$B$9:$B$109</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A104">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A12;A15;A9:A11;A13:A14;A16:A105">
       <formula1>PI!$A$9:$A$109</formula1>
     </dataValidation>
   </dataValidations>
@@ -3552,7 +4017,7 @@
   <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="7"/>
@@ -3564,116 +4029,116 @@
   </cols>
   <sheetData>
     <row r="1" ht="17.25" spans="1:8">
-      <c r="A1" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-    </row>
-    <row r="2" s="19" customFormat="1" ht="15" customHeight="1" spans="1:8">
+      <c r="A1" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+    </row>
+    <row r="2" s="21" customFormat="1" ht="15" customHeight="1" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="26"/>
-    </row>
-    <row r="3" s="19" customFormat="1" spans="1:8">
+      <c r="C2" s="15"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="27"/>
+    </row>
+    <row r="3" s="21" customFormat="1" spans="1:8">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="26"/>
-    </row>
-    <row r="4" s="19" customFormat="1" spans="1:8">
+      <c r="C3" s="16"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="27"/>
+    </row>
+    <row r="4" s="21" customFormat="1" spans="1:8">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="26"/>
-    </row>
-    <row r="5" s="19" customFormat="1" spans="1:8">
+      <c r="C4" s="16"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="27"/>
+    </row>
+    <row r="5" s="21" customFormat="1" spans="1:8">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="26"/>
-    </row>
-    <row r="6" s="19" customFormat="1" spans="1:8">
+      <c r="C5" s="16"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="27"/>
+    </row>
+    <row r="6" s="21" customFormat="1" spans="1:8">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="26"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="27"/>
     </row>
     <row r="7" spans="4:8">
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="23" t="str">
+      <c r="B8" s="25" t="str">
         <f>"AN"</f>
         <v>AN</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+        <v>139</v>
+      </c>
+      <c r="D8" s="26"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="19"/>
+      <c r="D9" s="21"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="25" t="s">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="25" t="s">
+      <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -4001,7 +4466,7 @@
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B109">
-      <formula1>AN!$B$9:$B$108</formula1>
+      <formula1>AN!$B$9:$B$109</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9;A10:A11;A12:A109">
       <formula1>PI!$A$9:$A$109</formula1>
@@ -4017,8 +4482,8 @@
   <sheetPr/>
   <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4037,21 +4502,21 @@
   <sheetData>
     <row r="1" ht="17.25" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>106</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="15" customHeight="1" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="13"/>
-      <c r="I2" s="17" t="s">
-        <v>108</v>
+      <c r="G2" s="15"/>
+      <c r="I2" s="19" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:9">
@@ -4061,9 +4526,9 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="14"/>
-      <c r="I3" s="18" t="s">
-        <v>109</v>
+      <c r="G3" s="16"/>
+      <c r="I3" s="20" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:9">
@@ -4073,9 +4538,9 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="14"/>
-      <c r="I4" s="18" t="s">
-        <v>110</v>
+      <c r="G4" s="16"/>
+      <c r="I4" s="20" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:7">
@@ -4085,7 +4550,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="14"/>
+      <c r="G5" s="16"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:7">
       <c r="A6" s="6"/>
@@ -4094,7 +4559,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="14"/>
+      <c r="G6" s="16"/>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:7">
       <c r="A7" s="6"/>
@@ -4103,7 +4568,7 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="14"/>
+      <c r="G7" s="16"/>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:7">
       <c r="A8" s="6"/>
@@ -4112,7 +4577,7 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="14"/>
+      <c r="G8" s="16"/>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:7">
       <c r="A9" s="8"/>
@@ -4121,7 +4586,7 @@
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="15"/>
+      <c r="G9" s="17"/>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:7">
       <c r="A10" s="7"/>
@@ -4134,151 +4599,371 @@
     </row>
     <row r="11" ht="25.5" spans="1:7">
       <c r="A11" s="10" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>115</v>
+        <v>149</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" ht="25.5" spans="1:7">
       <c r="A12" s="11" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>118</v>
+        <v>128</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="13" ht="25.5" spans="1:7">
       <c r="A13" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>101</v>
+        <v>142</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" ht="25.5" spans="1:7">
       <c r="A14" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>101</v>
+        <v>142</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" ht="25.5" spans="1:7">
       <c r="A15" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" ht="38.25" spans="1:7">
+      <c r="A16" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" ht="38.25" spans="1:7">
+      <c r="A17" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" ht="51" spans="1:7">
+      <c r="A18" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" ht="51" spans="1:7">
+      <c r="A19" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" ht="51" spans="1:7">
+      <c r="A20" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" ht="63.75" spans="1:7">
+      <c r="A21" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" ht="38.25" spans="1:7">
+      <c r="A22" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" ht="38.25" spans="1:7">
+      <c r="A23" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="24" ht="63.75" spans="1:7">
+      <c r="A24" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="11"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="11"/>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="11"/>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="11"/>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="11"/>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="11"/>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="11"/>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="11"/>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="11"/>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="11"/>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="11"/>
+      <c r="F24" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="25" ht="25.5" spans="1:7">
+      <c r="A25" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" ht="76.5" spans="1:7">
+      <c r="A26" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="11"/>
@@ -4533,24 +5218,25 @@
   <mergeCells count="1">
     <mergeCell ref="A2:G9"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F16:F109">
-      <formula1>ATVN!$C$9:$C$108</formula1>
+  <dataValidations count="7">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A16:A109"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12;F13:F15">
+      <formula1>EXPEC!$D$9:$D$101</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12;D13;D14;D15;D16:D109">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12;E16;E17;E18;E19;E20;E23;E13:E15;E21:E22;E24:E147">
+      <formula1>AFN!$C$9:$C$111</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12;D13;D14;D15;D16;D17;D18;D19;D20;D23;D24;D21:D22;D25:D109">
       <formula1>$I$2:$I$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12;E13:E15;E16:E147">
-      <formula1>AFN!$C$9:$C$110</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12;F13:F15">
-      <formula1>EXPEC!$D$9:$D$100</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12;A16:A107;C13:C15;C16:C112">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12;C16;C17;C18;C19;C20;C23;C24;C13:C15;C21:C22;C25:C112">
       <formula1>PI!$A$9:$A$109</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12;B13:B15;B16:B112">
-      <formula1>AN!$B$9:$B$108</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F16;F17;F18;F19;F20;F23;F21:F22;F24:F1048576">
+      <formula1>EXPEC!$D$9:$D$110</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12;B16;B17;B18;B19;B20;B23;B24;B13:B15;B21:B22;B25:B1048576">
+      <formula1>AN!$B$9:$B$109</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>

</xml_diff>